<commit_message>
Effects of age, gender and mental illness
Association of demographic, socioeconomic, accident-related and mental health parameters with age, gender and mental illness in the study cohort
</commit_message>
<xml_diff>
--- a/paper/supplementary_tables.xlsx
+++ b/paper/supplementary_tables.xlsx
@@ -11,6 +11,9 @@
     <sheet name="Supplementary Table S1" sheetId="2" r:id="rId2"/>
     <sheet name="Supplementary Table S2" sheetId="3" r:id="rId3"/>
     <sheet name="Supplementary Table S3" sheetId="4" r:id="rId4"/>
+    <sheet name="Supplementary Table S4" sheetId="5" r:id="rId5"/>
+    <sheet name="Supplementary Table S5" sheetId="6" r:id="rId6"/>
+    <sheet name="Supplementary Table S6" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -354,7 +357,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -404,7 +407,43 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Significant and near signifcant (unadjusted p &lt; 0.05) differences between individuals excluded from analysis and analyzed study participants. Numeric variables are presented as medians with interquartile ranges (IQR). Categorical variables are presented as percentages and counts within the complete observation set.</t>
+          <t>Significant and near significant (non-adjusted p &lt; 0.05) differences between individuals excluded from analysis and analyzed study participants. Numeric variables are presented as medians with interquartile ranges (IQR). Categorical variables are presented as percentages and counts within the complete observation set.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Supplementary Table S4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Significant and near significant (false discovery rate-adjusted p &lt; 0.1) demographic, socioeconomic, accident-related and mental health factors associated with age. Numeric variables are presented as medians with interquartile ranges (IQR). Categorical variables are presented as percentages and counts within the complete observation set.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Supplementary Table S5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Significant and near significant (false discovery rate-adjusted p &lt; 0.1) demographic, socioeconomic, accident-related and mental health factors associated with gender. Numeric variables are presented as medians with interquartile ranges (IQR). Categorical variables are presented as percentages and counts within the complete observation set.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Supplementary Table S6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Significant and near significant (false discovery rate-adjusted p &lt; 0.1) demographic, socioeconomic, accident-related and mental health factors associated with mental illness. Numeric variables are presented as medians with interquartile ranges (IQR). Categorical variables are presented as percentages and counts within the complete observation set.</t>
         </is>
       </c>
     </row>
@@ -415,7 +454,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C93"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -497,12 +536,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>weight</t>
+          <t>education</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Weight class</t>
+          <t>Highest education</t>
         </is>
       </c>
     </row>
@@ -514,12 +553,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>height</t>
+          <t>employment</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Height class</t>
+          <t>Employment status</t>
         </is>
       </c>
     </row>
@@ -531,12 +570,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>sport profession</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Highest education</t>
+          <t>Sport-related profession</t>
         </is>
       </c>
     </row>
@@ -548,12 +587,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>employment</t>
+          <t>trauma-risk profession</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Employment status</t>
+          <t>Trauma-risk profession</t>
         </is>
       </c>
     </row>
@@ -565,12 +604,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>sport profession</t>
+          <t>income/year</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Sport-related profession</t>
+          <t>Household income class per year</t>
         </is>
       </c>
     </row>
@@ -582,46 +621,46 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>trauma-risk profession</t>
+          <t>residence in the Alps</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Trauma-risk profession</t>
+          <t>Residence in an alpine region</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Demographics</t>
+          <t>Medical history</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>income/year</t>
+          <t>smoking</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Household income class per year</t>
+          <t>Smoking status</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Demographics</t>
+          <t>Medical history</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>residence in the Alps</t>
+          <t>smoking history</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Residence in an alpine region</t>
+          <t>Smoking history</t>
         </is>
       </c>
     </row>
@@ -633,12 +672,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>smoking</t>
+          <t>drug consumption</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Smoking status</t>
+          <t>Drug consumption</t>
         </is>
       </c>
     </row>
@@ -650,12 +689,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>smoking history</t>
+          <t>somatic comorbidity</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Smoking history</t>
+          <t>Somatic comorbidity</t>
         </is>
       </c>
     </row>
@@ -667,12 +706,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>drug consumption</t>
+          <t>somatic comorbidity type</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Drug consumption</t>
+          <t>Somatic comorbidity type</t>
         </is>
       </c>
     </row>
@@ -684,46 +723,46 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>somatic comorbidity</t>
+          <t>mental illness</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Somatic comorbidity</t>
+          <t>Mental comorbidity</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Medical history</t>
+          <t>Prior traumatic events</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>somatic comorbidity type</t>
+          <t>traumatic event before/DIA-X</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Somatic comorbidity type</t>
+          <t>Traumatic event prior to accident, DIA-X tool (also known as CIDI)</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Medical history</t>
+          <t>Prior traumatic events</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>mental illness</t>
+          <t>self-reported traumatic event type</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Mental comorbidity</t>
+          <t>Primary traumatic event type</t>
         </is>
       </c>
     </row>
@@ -735,63 +774,63 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>traumatic event before/DIA-X</t>
+          <t>self-reported traumatic event past</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Traumatic event prior to accident, DIA-X tool (also known as CIDI)</t>
+          <t>Time from the traumatic event</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Prior traumatic events</t>
+          <t>Alpine accident details</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>prior traumatic event number</t>
+          <t>prior sport accidents</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Traumatic event count, DIA-X score</t>
+          <t>Prior sport accidents</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Prior traumatic events</t>
+          <t>Alpine accident details</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>self-reported traumatic event type</t>
+          <t>accident year</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Primary traumatic event type</t>
+          <t>Year of the accident</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Prior traumatic events</t>
+          <t>Alpine accident details</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>self-reported traumatic event past</t>
+          <t>sport type</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Time from the traumatic event</t>
+          <t>Type of sport at the accident</t>
         </is>
       </c>
     </row>
@@ -803,12 +842,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>prior sport accidents</t>
+          <t>alone during the accident</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Prior sport accidents</t>
+          <t>Alone during the accident</t>
         </is>
       </c>
     </row>
@@ -820,12 +859,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>accident year</t>
+          <t>accident culprit</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Year of the accident</t>
+          <t>Accident culprit</t>
         </is>
       </c>
     </row>
@@ -837,12 +876,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>sport type</t>
+          <t>injured persons</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Type of sport at the accident</t>
+          <t>Accident injured persons</t>
         </is>
       </c>
     </row>
@@ -854,97 +893,97 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>alone during the accident</t>
+          <t>rescue</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Alone during the accident</t>
+          <t>Accident rescue</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Alpine accident details</t>
+          <t>Diagnosis and treatment</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>accident culprit</t>
+          <t>injury severity class</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Accident culprit</t>
+          <t>AIS injury severity grade</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Alpine accident details</t>
+          <t>Diagnosis and treatment</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>injured persons</t>
+          <t>head injury</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Accident injured persons</t>
+          <t>Head injury except of face</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Alpine accident details</t>
+          <t>Diagnosis and treatment</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>rescue</t>
+          <t>face injury</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Accident rescue</t>
+          <t>Face injury</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Alpine accident details</t>
+          <t>Diagnosis and treatment</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>rescue waiting time</t>
+          <t>neck injury</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Rescue waiting time</t>
+          <t>Neck injury</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Alpine accident details</t>
+          <t>Diagnosis and treatment</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>rescue mode</t>
+          <t>chest injury</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Rescue modality</t>
+          <t>Chest injury</t>
         </is>
       </c>
     </row>
@@ -956,12 +995,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>injury code</t>
+          <t>abdomen injury</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Code of the injury</t>
+          <t>Abdomen injury</t>
         </is>
       </c>
     </row>
@@ -973,24 +1012,29 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>injury severity</t>
+          <t>spine region injury</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>AIS injury severity grade</t>
+          <t>Spine region injury</t>
         </is>
       </c>
     </row>
     <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Diagnosis and treatment</t>
+        </is>
+      </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>injury severity class</t>
+          <t>upper limb injury</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>AIS injury severity grade</t>
+          <t>Hand, arm or shoulder injury</t>
         </is>
       </c>
     </row>
@@ -1002,12 +1046,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>head injury</t>
+          <t>lower limb injury</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Head injury except of face</t>
+          <t>Leg, foot or hip injury</t>
         </is>
       </c>
     </row>
@@ -1019,12 +1063,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>face injury</t>
+          <t>other injury</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Face injury</t>
+          <t>Other external injury</t>
         </is>
       </c>
     </row>
@@ -1036,284 +1080,284 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>neck injury</t>
+          <t>psychological support</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Neck injury</t>
+          <t>Psychological support after the accident</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Diagnosis and treatment</t>
+          <t>Alpine accident outcome</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>chest injury</t>
+          <t>somatic accident aftermath</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Chest injury</t>
+          <t>Accident consequences felt, somatic health</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Diagnosis and treatment</t>
+          <t>Alpine accident outcome</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>abdomen injury</t>
+          <t>returned to same sport</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Abdomen injury</t>
+          <t>Returned to the same sport activity post accident</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Diagnosis and treatment</t>
+          <t>Alpine accident outcome</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>spine region injury</t>
+          <t>behavior post accident</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Spine region injury</t>
+          <t>Behavior after accident</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Diagnosis and treatment</t>
+          <t>Alpine accident outcome</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>upper limb injury</t>
+          <t>flashbacks during sport</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Hand, arm or shoulder injury</t>
+          <t>Flashback during sport activity</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Diagnosis and treatment</t>
+          <t>Alpine accident outcome</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>lower limb injury</t>
+          <t>flashback frequency</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Leg, foot or hip injury</t>
+          <t>Flashback frequency</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Diagnosis and treatment</t>
+          <t>Alpine accident outcome</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>other injury</t>
+          <t>confusion during sport</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Other external injury</t>
+          <t>Confusion during sport activity</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Diagnosis and treatment</t>
+          <t>PTSD assessment</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>psych. support need</t>
+          <t>PCL-5 DSM-5 score</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Psychological support needed, self-report</t>
+          <t>PTSD rating, PCL-5 DSM-5</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Diagnosis and treatment</t>
+          <t>PTSD assessment</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>psychological support</t>
+          <t>PTSD+ (PCL-5 DSM-5 &gt;31)</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Psychological support after the accident</t>
+          <t>PTSD symptoms, PCL-5 DSM5</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Diagnosis and treatment</t>
+          <t>PTSD assessment</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>psych. support assessment</t>
+          <t>PTSD+ (at least one cluster)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Psychological support assessment</t>
+          <t>At least one PCL-5 DSM-5 cluster positive</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Diagnosis and treatment</t>
+          <t>PTSD assessment</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>psychological therapy post accident</t>
+          <t>PCL-5 DSM-5 cluster B score</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Psychological /psychiatric therapy after the accident</t>
+          <t>PTSD rating, PCL-5 DSM-5 cluster B</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Alpine accident outcome</t>
+          <t>PTSD assessment</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>somatic accident aftermath</t>
+          <t>PTSD cluster B+</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Accident consequences felt, somatic health</t>
+          <t>PTSD symptoms, PCL-5 DSM-5 cluster B positive</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Alpine accident outcome</t>
+          <t>PTSD assessment</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>returned to same sport</t>
+          <t>PCL-5 DSM-5 cluster C score</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Returned to the same sport activity post accident</t>
+          <t>PTSD rating, PCL-5 DSM-5 cluster C</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Alpine accident outcome</t>
+          <t>PTSD assessment</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>behavior post accident</t>
+          <t>PTSD cluster C+</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Behavior after accident</t>
+          <t>PTSD symptoms, PCL-5 DSM-5 cluster C positive</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Alpine accident outcome</t>
+          <t>PTSD assessment</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>flashbacks during sport</t>
+          <t>PCL-5 DSM-5 cluster D score</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Flashback during sport activity</t>
+          <t>PTSD rating, PCL-5 DSM-5 cluster D</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Alpine accident outcome</t>
+          <t>PTSD assessment</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>flashback frequency</t>
+          <t>PTSD cluster D+</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Flashback frequency</t>
+          <t>PTSD symptoms, PCL-5 DSM-5 cluster D positive</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Alpine accident outcome</t>
+          <t>PTSD assessment</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>confusion during sport</t>
+          <t>PCL-5 DSM-5 cluster E score</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Confusion during sport activity</t>
+          <t>PTSD rating, PCL-5 DSM-5 cluster E</t>
         </is>
       </c>
     </row>
@@ -1325,673 +1369,503 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>PCL-5 DSM-5 score</t>
+          <t>PTSD cluster E+</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>PTSD rating, PCL-5 DSM-5</t>
+          <t>PTSD symptoms, PCL-5 DSM-5 cluster E positive</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>PTSD assessment</t>
+          <t>PTG assessment</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>PTSD+ (PCL-5 DSM-5 &gt;31)</t>
+          <t>PTGI score</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>PTSD symptoms, PCL-5 DSM5</t>
+          <t>PTGI scoring</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>PTSD assessment</t>
+          <t>PTG assessment</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>PTSD+ (at least one cluster)</t>
+          <t>PTGI I relations score</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>At least one PCL-5 DSM-5 cluster positive</t>
+          <t>PTGI scoring, factor I, relations</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>PTSD assessment</t>
+          <t>PTG assessment</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>PCL-5 DSM-5 cluster B score</t>
+          <t>PTGI II possibilities score</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>PTSD rating, PCL-5 DSM-5 cluster B</t>
+          <t>PTGI scoring, factor II, new possibilities</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>PTSD assessment</t>
+          <t>PTG assessment</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>PTSD cluster B+</t>
+          <t>PTGI III personal strength score</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>PTSD symptoms, PCL-5 DSM-5 cluster B positive</t>
+          <t>PTGI scoring, factor III, personal strength</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>PTSD assessment</t>
+          <t>PTG assessment</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>PCL-5 DSM-5 cluster C score</t>
+          <t>PTGI IV spiritual score</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>PTSD rating, PCL-5 DSM-5 cluster C</t>
+          <t>PTGI scoring, factor IV, spiritual</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>PTSD assessment</t>
+          <t>PTG assessment</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>PTSD cluster C+</t>
+          <t>PTGI V life appreciation score</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>PTSD symptoms, PCL-5 DSM-5 cluster C positive</t>
+          <t>PTGI scoring, factor V, appreciation of life</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>PTSD assessment</t>
+          <t>Resilient coping</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>PCL-5 DSM-5 cluster D score</t>
+          <t>RS13 score</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>PTSD rating, PCL-5 DSM-5 cluster D</t>
+          <t>RS13 score</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>PTSD assessment</t>
+          <t>Resilient coping</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>PTSD cluster D+</t>
+          <t>RS13 coping class</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>PTSD symptoms, PCL-5 DSM-5 cluster D positive</t>
+          <t>RS13 coping class</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>PTSD assessment</t>
+          <t>Alcohol and drug abuse</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>PCL-5 DSM-5 cluster E score</t>
+          <t>CAGE score</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>PTSD rating, PCL-5 DSM-5 cluster E</t>
+          <t>CAGE score</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>PTSD assessment</t>
+          <t>Alcohol and drug abuse</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>PTSD cluster E+</t>
+          <t>Abuse+ (CAGE ≥2)</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>PTSD symptoms, PCL-5 DSM-5 cluster E positive</t>
+          <t>Abuse+ (CAGE ≥2)</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>PTG assessment</t>
+          <t>Psychosocial stress</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>PTGI score</t>
+          <t>PSS4 score</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>PTGI scoring</t>
+          <t>PSS4 score</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>PTG assessment</t>
+          <t>Sense of coherence</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>PTGI I relations score</t>
+          <t>SOC-9L score</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>PTGI scoring, factor I, relations</t>
+          <t>SOC-9L score</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>PTG assessment</t>
+          <t>PHQ mental health</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>PTGI II possibilities score</t>
+          <t>PHQ-9 score</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>PTGI scoring, factor II, new possibilities</t>
+          <t>PHQ-9 score, depression</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>PTG assessment</t>
+          <t>PHQ mental health</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>PTGI III personal strength score</t>
+          <t>Depression+ (PHQ-9 ≥11)</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>PTGI scoring, factor III, personal strength</t>
+          <t>PHQ-9 score, depression signs</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>PTG assessment</t>
+          <t>PHQ mental health</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>PTGI IV spiritual score</t>
+          <t>GAD-7 score</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>PTGI scoring, factor IV, spiritual</t>
+          <t>GAD-7 score, anxiety</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>PTG assessment</t>
+          <t>PHQ mental health</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>PTGI V life appreciation score</t>
+          <t>Anxiety+ (GAD-7 ≥10)</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>PTGI scoring, factor V, appreciation of life</t>
+          <t>GAD-7 score, anxiety signs</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Resilient coping</t>
+          <t>PHQ mental health</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>RS13 score</t>
+          <t>PHQ-panic score</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>RS13 score</t>
+          <t>PHQ panic 4 item score</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Resilient coping</t>
+          <t>PHQ mental health</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>RS13 coping class</t>
+          <t>Panic+ (PHQ-panic)</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>RS13 coping class</t>
+          <t>PHQ panic positivity</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Alcohol and drug abuse</t>
+          <t>PHQ mental health</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>CAGE score</t>
+          <t>PHQ-15 score</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>CAGE score</t>
+          <t>PHQ-15 health problems, somatization</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Alcohol and drug abuse</t>
+          <t>PHQ mental health</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Abuse+ (CAGE ≥2)</t>
+          <t>Somatization+ (PHQ-15 ≥11)</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Abuse+ (CAGE ≥2)</t>
+          <t>PHQ-15 health problems, moderate-severe symptoms</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Psychosocial stress</t>
+          <t>Quality of life</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>PSS4 score</t>
+          <t>EUROHIS-QOL 8 score</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>PSS4 score</t>
+          <t>EUROHIS-QOL 8 score</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Sense of coherence</t>
+          <t>Quality of life</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>SOC-9L score</t>
+          <t>EUROHIS-QOL 8 QoL score</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>SOC-9L score</t>
+          <t>EUROHIS-QOL 8 score QoL problems</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>PHQ mental health</t>
+          <t>Quality of life</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>PHQ-9 score</t>
+          <t>EUROHIS-QOL 8 health score</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>PHQ-9 score, depression</t>
+          <t>EUROHIS-QOL 8 score health problems</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>PHQ mental health</t>
+          <t>Quality of life</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Depression+ (PHQ-9 ≥11)</t>
+          <t>EUROHIS-QOL 8 energy score</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>PHQ-9 score, depression signs</t>
+          <t>EUROHIS-QOL 8 score energy problems</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>PHQ mental health</t>
+          <t>Quality of life</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>GAD-7 score</t>
+          <t>EUROHIS-QOL 8 finances score</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>GAD-7 score, anxiety</t>
+          <t>EUROHIS-QOL 8 score financial problems</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>PHQ mental health</t>
+          <t>Quality of life</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Anxiety+ (GAD-7 ≥10)</t>
+          <t>EUROHIS-QOL 8 activity score</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>GAD-7 score, anxiety signs</t>
+          <t>EUROHIS-QOL 8 score activity problems</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>PHQ mental health</t>
+          <t>Quality of life</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>PHQ-panic score</t>
+          <t>EUROHIS-QOL 8 self-esteem score</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>PHQ panic 4 item score</t>
+          <t>EUROHIS-QOL 8 score self-esteem problems</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>PHQ mental health</t>
+          <t>Quality of life</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Panic+ (PHQ-panic)</t>
+          <t>EUROHIS-QOL 8 relationship score</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>PHQ panic positivity</t>
+          <t>EUROHIS-QOL 8 score relationship problems</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>PHQ mental health</t>
+          <t>Quality of life</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>PHQ-15 score</t>
+          <t>EUROHIS-QOL 8 housing score</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
-        <is>
-          <t>PHQ-15 health problems, somatization</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>PHQ mental health</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>Somatization+ (PHQ-15 ≥11)</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>PHQ-15 health problems, moderate-severe symptoms</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>Quality of life</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>EUROHIS-QOL 8 score</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>EUROHIS-QOL 8 score</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>Quality of life</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>EUROHIS-QOL 8 QoL score</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>EUROHIS-QOL 8 score QoL problems</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>Quality of life</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>EUROHIS-QOL 8 health score</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>EUROHIS-QOL 8 score health problems</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>Quality of life</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>EUROHIS-QOL 8 energy score</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>EUROHIS-QOL 8 score energy problems</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>Quality of life</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>EUROHIS-QOL 8 finances score</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>EUROHIS-QOL 8 score financial problems</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>Quality of life</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>EUROHIS-QOL 8 activity score</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>EUROHIS-QOL 8 score activity problems</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>Quality of life</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>EUROHIS-QOL 8 self-esteem score</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>EUROHIS-QOL 8 score self-esteem problems</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>Quality of life</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>EUROHIS-QOL 8 relationship score</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>EUROHIS-QOL 8 score relationship problems</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>Quality of life</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>EUROHIS-QOL 8 housing score</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
         <is>
           <t>EUROHIS-QOL 8 score housing problems</t>
         </is>
@@ -2714,7 +2588,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2775,7 +2649,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ns (p = 0.12)</t>
+          <t>ns (p = 0.11)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -2812,7 +2686,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>p = 0.029</t>
+          <t>p = 0.026</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -2824,41 +2698,10 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>injury severity, AIS score</t>
+          <t>injury severity class, AIS score</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
-        <is>
-          <t>2 [IQR: 1 - 3]
-range: 1 - 5
-n = 279</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2 [IQR: 1 - 2]
-range: 1 - 4
-n = 70</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>ns (p = 0.24)</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>r = 0.12</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>injury severity class, AIS score</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
         <is>
           <t>1: 37% (n = 104)
 2: 33% (n = 93)
@@ -2866,7 +2709,7 @@
 n = 279</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>1: 46% (n = 32)
 2: 40% (n = 28)
@@ -2874,38 +2717,67 @@
 n = 70</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>ns (p = 0.23)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>V = 0.14</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>upper limb injury</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>42% (n = 118)
+n = 279</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>57% (n = 40)
+n = 70</t>
+        </is>
+      </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>ns (p = 0.24)</t>
+          <t>ns (p = 0.23)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>V = 0.14</t>
+          <t>V = 0.12</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>upper limb injury</t>
+          <t>somatic accident aftermath</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>42% (n = 118)
-n = 279</t>
+          <t>37% (n = 115)
+n = 307</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>57% (n = 40)
-n = 70</t>
+          <t>22% (n = 12)
+n = 55</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ns (p = 0.24)</t>
+          <t>ns (p = 0.23)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -2917,215 +2789,1117 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>somatic accident aftermath</t>
+          <t>PTGI score</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
-        <is>
-          <t>37% (n = 115)
-n = 307</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>22% (n = 12)
-n = 55</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>ns (p = 0.24)</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>V = 0.12</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>PTGI score</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
         <is>
           <t>32 [IQR: 16 - 48]
 range: 0 - 100
 n = 307</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>8.5 [IQR: 3 - 41]
 range: 0 - 78
 n = 18</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>ns (p = 0.24)</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>ns (p = 0.23)</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>r = 0.12</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+    <row r="8">
+      <c r="A8" t="inlineStr">
         <is>
           <t>PTGI I relations score</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>12 [IQR: 6 - 18]
 range: 0 - 35
 n = 307</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>2.5 [IQR: 0 - 13]
 range: 0 - 28
 n = 18</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>ns (p = 0.12)</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>ns (p = 0.11)</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>r = 0.15</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+    <row r="9">
+      <c r="A9" t="inlineStr">
         <is>
           <t>PTGI III personal strength score</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>8 [IQR: 4 - 11]
 range: 0 - 20
 n = 307</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>4.5 [IQR: 0 - 8.8]
 range: 0 - 16
 n = 18</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>ns (p = 0.24)</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>ns (p = 0.23)</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>r = 0.12</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+    <row r="10">
+      <c r="A10" t="inlineStr">
         <is>
           <t>PTGI V life appreciation score</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>6 [IQR: 2 - 9]
 range: 0 - 15
 n = 307</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>1.5 [IQR: 0.25 - 6.8]
 range: 0 - 12
 n = 18</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>ns (p = 0.27)</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>ns (p = 0.28)</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
         <is>
           <t>r = 0.11</t>
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+    <row r="11">
+      <c r="A11" t="inlineStr">
         <is>
           <t>PSS4 score</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>4 [IQR: 3 - 6]
 range: 0 - 14
 n = 307</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>5.5 [IQR: 4 - 7]
 range: 0 - 9
 n = 42</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>ns (p = 0.24)</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>ns (p = 0.23)</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>r = 0.12</t>
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+    <row r="12">
+      <c r="A12" t="inlineStr">
         <is>
           <t>SOC-9L score</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>19 [IQR: 16 - 25]
 range: 10 - 49
 n = 307</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>27 [IQR: 20 - 35]
 range: 17 - 50
 n = 11</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>ns (p = 0.12)</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>ns (p = 0.11)</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>r = 0.15</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Variable</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Young adult</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Middle-aged</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Elderly</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>significance (FDR)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Effect size</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>employment</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>employed: 54% (n = 33)
+household: 0% (n = 0)
+unemployed: 0% (n = 0)
+student: 46% (n = 28)
+retired: 0% (n = 0)
+n = 61</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>employed: 85% (n = 172)
+household: 3.5% (n = 7)
+unemployed: 0.5% (n = 1)
+student: 1.5% (n = 3)
+retired: 9.4% (n = 19)
+n = 202</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>employed: 11% (n = 5)
+household: 6.8% (n = 3)
+unemployed: 0% (n = 0)
+student: 2.3% (n = 1)
+retired: 80% (n = 35)
+n = 44</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>V = 0.63</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>income/year</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>no income: 18% (n = 11)
+&lt; 15000 Euro: 16% (n = 10)
+15000 - 30000 Euro: 21% (n = 13)
+30000 - 45000 Euro: 18% (n = 11)
+&gt; 45000 Euro: 26% (n = 16)
+n = 61</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>no income: 19% (n = 38)
+&lt; 15000 Euro: 3% (n = 6)
+15000 - 30000 Euro: 10% (n = 21)
+30000 - 45000 Euro: 19% (n = 38)
+&gt; 45000 Euro: 49% (n = 99)
+n = 202</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>no income: 32% (n = 14)
+&lt; 15000 Euro: 2.3% (n = 1)
+15000 - 30000 Euro: 11% (n = 5)
+30000 - 45000 Euro: 23% (n = 10)
+&gt; 45000 Euro: 32% (n = 14)
+n = 44</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>p = 0.0033</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>V = 0.23</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>alone during the accident</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>15% (n = 9)
+n = 61</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>33% (n = 67)
+n = 202</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>48% (n = 21)
+n = 44</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>p = 0.019</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>V = 0.21</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>rescue</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>self: 57% (n = 35)
+tour partner: 8.2% (n = 5)
+rescue team: 30% (n = 18)
+third party: 4.9% (n = 3)
+n = 61</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>self: 51% (n = 104)
+tour partner: 14% (n = 29)
+rescue team: 29% (n = 58)
+third party: 5.4% (n = 11)
+n = 202</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>self: 36% (n = 16)
+tour partner: 11% (n = 5)
+rescue team: 30% (n = 13)
+third party: 23% (n = 10)
+n = 44</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>ns (p = 0.06)</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>V = 0.17</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>PTGI V life appreciation score</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>4 [IQR: 0 - 7]
+range: 0 - 15
+n = 61</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>7 [IQR: 3 - 9]
+range: 0 - 15
+n = 202</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>5 [IQR: 2 - 8.2]
+range: 0 - 13
+n = 44</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>ns (p = 0.06)</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>η² = 0.028</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SOC-9L score</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>22 [IQR: 20 - 31]
+range: 11 - 41
+n = 61</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>18 [IQR: 16 - 23]
+range: 10 - 49
+n = 202</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>19 [IQR: 16 - 21]
+range: 13 - 31
+n = 44</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>η² = 0.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>PHQ-panic score</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0]
+range: 0 - 4
+n = 61</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0]
+range: 0 - 4
+n = 202</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0]
+range: 0 - 2
+n = 44</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>p = 0.0079</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>η² = 0.045</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>EUROHIS-QOL 8 housing score</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1 [IQR: 1 - 2]
+range: 1 - 5
+n = 61</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1 [IQR: 1 - 2]
+range: 1 - 5
+n = 202</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1 [IQR: 1 - 1]
+range: 1 - 5
+n = 44</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>ns (p = 0.06)</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>η² = 0.027</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Variable</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Significance (FDR)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Effect size</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>income/year</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>no income: 25% (n = 34)
+&lt; 15000 Euro: 8% (n = 11)
+15000 - 30000 Euro: 17% (n = 23)
+30000 - 45000 Euro: 20% (n = 27)
+&gt; 45000 Euro: 31% (n = 42)
+n = 137</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>no income: 17% (n = 29)
+&lt; 15000 Euro: 3.5% (n = 6)
+15000 - 30000 Euro: 9.4% (n = 16)
+30000 - 45000 Euro: 19% (n = 32)
+&gt; 45000 Euro: 51% (n = 87)
+n = 170</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ns (p = 0.052)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>V = 0.23</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>upper limb injury</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>33% (n = 42)
+n = 126</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>50% (n = 76)
+n = 153</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>ns (p = 0.1)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>V = 0.16</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>PCL-5 DSM-5 cluster C score</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 1]
+range: 0 - 8
+n = 137</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0]
+range: 0 - 5
+n = 170</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>p = 0.037</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>r = 0.18</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>PTGI score</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>35 [IQR: 24 - 52]
+range: 0 - 100
+n = 137</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>28 [IQR: 10 - 45]
+range: 0 - 94
+n = 170</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>p = 0.037</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>r = 0.18</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>PTGI I relations score</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>14 [IQR: 9 - 20]
+range: 0 - 35
+n = 137</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>11 [IQR: 5 - 17]
+range: 0 - 34
+n = 170</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>ns (p = 0.082)</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>r = 0.16</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>PTGI III personal strength score</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>9 [IQR: 6 - 12]
+range: 0 - 20
+n = 137</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>7 [IQR: 2 - 11]
+range: 0 - 19
+n = 170</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>p = 0.031</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>r = 0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>PTGI V life appreciation score</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>7 [IQR: 4 - 9]
+range: 0 - 15
+n = 137</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>4 [IQR: 1.2 - 8]
+range: 0 - 15
+n = 170</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>p = 0.037</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>r = 0.18</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Variable</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>No mental illness</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Mental illness</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Significance (FDR)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Effect size</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>smoking</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>6.9% (n = 20)
+n = 291</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>25% (n = 4)
+n = 16</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ns (p = 0.094)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>V = 0.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>smoking history, years</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0]
+range: 0 - 50
+n = 291</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 2.5]
+range: 0 - 30
+n = 16</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>p = 0.034</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>r = 0.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>self-reported traumatic event type</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>none: 89% (n = 259)
+severe accident: 6.5% (n = 19)
+physical assult: 1.4% (n = 4)
+sexual molestation: 0.69% (n = 2)
+rape: 0% (n = 0)
+severe disease: 1.7% (n = 5)
+natural diseaster: 0.34% (n = 1)
+war: 0.34% (n = 1)
+n = 291</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>none: 75% (n = 12)
+severe accident: 0% (n = 0)
+physical assult: 6.2% (n = 1)
+sexual molestation: 0% (n = 0)
+rape: 6.2% (n = 1)
+severe disease: 6.2% (n = 1)
+natural diseaster: 6.2% (n = 1)
+war: 0% (n = 0)
+n = 16</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>V = 0.32</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>flashbacks during sport</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>37% (n = 108)
+n = 291</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>88% (n = 14)
+n = 16</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>V = 0.23</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>flashback frequency</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>no flashbacks: 63% (n = 183)
+&gt; 1 – 2 per week: 2.7% (n = 8)
+several per month: 4.8% (n = 14)
+1 – 2 per month: 8.9% (n = 26)
+1 – 2 per year: 21% (n = 60)
+n = 291</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>no flashbacks: 12% (n = 2)
+&gt; 1 – 2 per week: 0% (n = 0)
+several per month: 12% (n = 2)
+1 – 2 per month: 25% (n = 4)
+1 – 2 per year: 50% (n = 8)
+n = 16</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>p = 0.0039</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>V = 0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>PCL-5 DSM-5 score</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>3 [IQR: 1 - 6]
+range: 0 - 44
+n = 291</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>10 [IQR: 3.8 - 18]
+range: 0 - 29
+n = 16</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>p = 0.0053</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>r = 0.18</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>PTSD+ (at least one cluster)</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>18% (n = 51)
+n = 291</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>44% (n = 7)
+n = 16</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>ns (p = 0.07)</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>V = 0.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>EUROHIS-QOL 8 score</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1.6 [IQR: 1.4 - 1.9]
+range: 1 - 4
+n = 291</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2.5 [IQR: 2.2 - 2.8]
+range: 1.4 - 3.2
+n = 16</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>r = 0.27</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
clustTools and caretExtra compatibility
Compatibility with the newest package versions and new tools
</commit_message>
<xml_diff>
--- a/paper/supplementary_tables.xlsx
+++ b/paper/supplementary_tables.xlsx
@@ -849,7 +849,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -883,15 +883,10 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Brier skill score</t>
+          <t>Sensitivity, PTS cluster</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Sensitivity, PTS cluster</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Specificity, PTS cluster</t>
         </is>
@@ -918,14 +913,11 @@
         <v>0.15</v>
       </c>
       <c r="F2">
-        <v>0.88</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -945,15 +937,12 @@
         <v>0.11</v>
       </c>
       <c r="E3">
-        <v>0.67</v>
+        <v>0.68</v>
       </c>
       <c r="F3">
-        <v>0.48</v>
+        <v>0.42</v>
       </c>
       <c r="G3">
-        <v>0.42</v>
-      </c>
-      <c r="H3">
         <v>0.68</v>
       </c>
     </row>
@@ -978,12 +967,9 @@
         <v>0.66</v>
       </c>
       <c r="F4">
-        <v>0.52</v>
+        <v>0.48</v>
       </c>
       <c r="G4">
-        <v>0.48</v>
-      </c>
-      <c r="H4">
         <v>0.68</v>
       </c>
     </row>
@@ -1008,14 +994,11 @@
         <v>0.018</v>
       </c>
       <c r="F5">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1038,12 +1021,9 @@
         <v>0.88</v>
       </c>
       <c r="F6">
-        <v>0.34</v>
+        <v>0.35</v>
       </c>
       <c r="G6">
-        <v>0.35</v>
-      </c>
-      <c r="H6">
         <v>0.6899999999999999</v>
       </c>
     </row>
@@ -1068,12 +1048,9 @@
         <v>0.96</v>
       </c>
       <c r="F7">
-        <v>0.32</v>
+        <v>0.33</v>
       </c>
       <c r="G7">
-        <v>0.33</v>
-      </c>
-      <c r="H7">
         <v>0.72</v>
       </c>
     </row>
@@ -1098,12 +1075,9 @@
         <v>0.57</v>
       </c>
       <c r="F8">
-        <v>0.52</v>
+        <v>0.88</v>
       </c>
       <c r="G8">
-        <v>0.88</v>
-      </c>
-      <c r="H8">
         <v>0.99</v>
       </c>
     </row>
@@ -1128,12 +1102,9 @@
         <v>0.67</v>
       </c>
       <c r="F9">
-        <v>0.48</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="G9">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="H9">
         <v>0.59</v>
       </c>
     </row>
@@ -1158,12 +1129,9 @@
         <v>0.66</v>
       </c>
       <c r="F10">
-        <v>0.55</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="G10">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="H10">
         <v>0.64</v>
       </c>
     </row>
@@ -1188,12 +1156,9 @@
         <v>0.5</v>
       </c>
       <c r="F11">
-        <v>0.61</v>
+        <v>0.62</v>
       </c>
       <c r="G11">
-        <v>0.62</v>
-      </c>
-      <c r="H11">
         <v>0.84</v>
       </c>
     </row>
@@ -1218,12 +1183,9 @@
         <v>0.77</v>
       </c>
       <c r="F12">
-        <v>0.44</v>
+        <v>0.38</v>
       </c>
       <c r="G12">
-        <v>0.38</v>
-      </c>
-      <c r="H12">
         <v>0.76</v>
       </c>
     </row>
@@ -1248,12 +1210,9 @@
         <v>0.78</v>
       </c>
       <c r="F13">
-        <v>0.41</v>
+        <v>0.33</v>
       </c>
       <c r="G13">
-        <v>0.33</v>
-      </c>
-      <c r="H13">
         <v>0.7</v>
       </c>
     </row>
@@ -1278,12 +1237,9 @@
         <v>0.41</v>
       </c>
       <c r="F14">
-        <v>0.7</v>
+        <v>0.68</v>
       </c>
       <c r="G14">
-        <v>0.68</v>
-      </c>
-      <c r="H14">
         <v>0.87</v>
       </c>
     </row>
@@ -1308,12 +1264,9 @@
         <v>0.8</v>
       </c>
       <c r="F15">
-        <v>0.42</v>
+        <v>0.38</v>
       </c>
       <c r="G15">
-        <v>0.38</v>
-      </c>
-      <c r="H15">
         <v>0.68</v>
       </c>
     </row>
@@ -1338,12 +1291,9 @@
         <v>0.74</v>
       </c>
       <c r="F16">
-        <v>0.41</v>
+        <v>0.33</v>
       </c>
       <c r="G16">
-        <v>0.33</v>
-      </c>
-      <c r="H16">
         <v>0.68</v>
       </c>
     </row>
@@ -1368,12 +1318,9 @@
         <v>0.55</v>
       </c>
       <c r="F17">
-        <v>0.57</v>
+        <v>0.75</v>
       </c>
       <c r="G17">
-        <v>0.75</v>
-      </c>
-      <c r="H17">
         <v>0.84</v>
       </c>
     </row>
@@ -1398,12 +1345,9 @@
         <v>0.66</v>
       </c>
       <c r="F18">
-        <v>0.52</v>
+        <v>0.4</v>
       </c>
       <c r="G18">
-        <v>0.4</v>
-      </c>
-      <c r="H18">
         <v>0.67</v>
       </c>
     </row>
@@ -1428,12 +1372,9 @@
         <v>0.65</v>
       </c>
       <c r="F19">
-        <v>0.44</v>
+        <v>0.48</v>
       </c>
       <c r="G19">
-        <v>0.48</v>
-      </c>
-      <c r="H19">
         <v>0.74</v>
       </c>
     </row>
@@ -1458,12 +1399,9 @@
         <v>0.41</v>
       </c>
       <c r="F20">
-        <v>0.7</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="G20">
-        <v>0.6899999999999999</v>
-      </c>
-      <c r="H20">
         <v>0.86</v>
       </c>
     </row>
@@ -1488,12 +1426,9 @@
         <v>0.76</v>
       </c>
       <c r="F21">
-        <v>0.4</v>
+        <v>0.38</v>
       </c>
       <c r="G21">
-        <v>0.38</v>
-      </c>
-      <c r="H21">
         <v>0.66</v>
       </c>
     </row>
@@ -1518,12 +1453,9 @@
         <v>0.74</v>
       </c>
       <c r="F22">
-        <v>0.52</v>
+        <v>0.41</v>
       </c>
       <c r="G22">
-        <v>0.41</v>
-      </c>
-      <c r="H22">
         <v>0.62</v>
       </c>
     </row>
@@ -1534,7 +1466,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1568,15 +1500,10 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Brier skill score</t>
+          <t>Sensitivity, PTS cluster</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Sensitivity, PTS cluster</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Specificity, PTS cluster</t>
         </is>
@@ -1603,12 +1530,9 @@
         <v>0.42</v>
       </c>
       <c r="F2">
-        <v>0.68</v>
+        <v>0.95</v>
       </c>
       <c r="G2">
-        <v>0.95</v>
-      </c>
-      <c r="H2">
         <v>0.98</v>
       </c>
     </row>
@@ -1633,12 +1557,9 @@
         <v>0.65</v>
       </c>
       <c r="F3">
-        <v>0.5</v>
+        <v>0.48</v>
       </c>
       <c r="G3">
-        <v>0.48</v>
-      </c>
-      <c r="H3">
         <v>0.68</v>
       </c>
     </row>
@@ -1663,12 +1584,9 @@
         <v>0.64</v>
       </c>
       <c r="F4">
-        <v>0.5</v>
+        <v>0.52</v>
       </c>
       <c r="G4">
-        <v>0.52</v>
-      </c>
-      <c r="H4">
         <v>0.7</v>
       </c>
     </row>
@@ -1693,12 +1611,9 @@
         <v>0.18</v>
       </c>
       <c r="F5">
-        <v>0.87</v>
+        <v>0.91</v>
       </c>
       <c r="G5">
-        <v>0.91</v>
-      </c>
-      <c r="H5">
         <v>1</v>
       </c>
     </row>
@@ -1723,12 +1638,9 @@
         <v>0.9</v>
       </c>
       <c r="F6">
-        <v>0.28</v>
+        <v>0.48</v>
       </c>
       <c r="G6">
-        <v>0.48</v>
-      </c>
-      <c r="H6">
         <v>0.75</v>
       </c>
     </row>
@@ -1753,12 +1665,9 @@
         <v>0.92</v>
       </c>
       <c r="F7">
-        <v>0.28</v>
+        <v>0.3</v>
       </c>
       <c r="G7">
-        <v>0.3</v>
-      </c>
-      <c r="H7">
         <v>0.85</v>
       </c>
     </row>
@@ -1783,12 +1692,9 @@
         <v>0.52</v>
       </c>
       <c r="F8">
-        <v>0.59</v>
+        <v>0.75</v>
       </c>
       <c r="G8">
-        <v>0.75</v>
-      </c>
-      <c r="H8">
         <v>0.8</v>
       </c>
     </row>
@@ -1813,12 +1719,9 @@
         <v>0.63</v>
       </c>
       <c r="F9">
-        <v>0.5</v>
+        <v>0.59</v>
       </c>
       <c r="G9">
-        <v>0.59</v>
-      </c>
-      <c r="H9">
         <v>0.68</v>
       </c>
     </row>
@@ -1843,12 +1746,9 @@
         <v>0.64</v>
       </c>
       <c r="F10">
-        <v>0.54</v>
+        <v>0.48</v>
       </c>
       <c r="G10">
-        <v>0.48</v>
-      </c>
-      <c r="H10">
         <v>0.7</v>
       </c>
     </row>
@@ -1876,9 +1776,6 @@
         <v>0.55</v>
       </c>
       <c r="G11">
-        <v>0.55</v>
-      </c>
-      <c r="H11">
         <v>0.79</v>
       </c>
     </row>
@@ -1903,12 +1800,9 @@
         <v>0.7</v>
       </c>
       <c r="F12">
-        <v>0.46</v>
+        <v>0.39</v>
       </c>
       <c r="G12">
-        <v>0.39</v>
-      </c>
-      <c r="H12">
         <v>0.66</v>
       </c>
     </row>
@@ -1933,12 +1827,9 @@
         <v>0.7</v>
       </c>
       <c r="F13">
-        <v>0.36</v>
+        <v>0.41</v>
       </c>
       <c r="G13">
-        <v>0.41</v>
-      </c>
-      <c r="H13">
         <v>0.72</v>
       </c>
     </row>
@@ -1963,12 +1854,9 @@
         <v>0.34</v>
       </c>
       <c r="F14">
-        <v>0.74</v>
+        <v>0.71</v>
       </c>
       <c r="G14">
-        <v>0.71</v>
-      </c>
-      <c r="H14">
         <v>0.88</v>
       </c>
     </row>
@@ -1996,9 +1884,6 @@
         <v>0.42</v>
       </c>
       <c r="G15">
-        <v>0.42</v>
-      </c>
-      <c r="H15">
         <v>0.77</v>
       </c>
     </row>
@@ -2023,12 +1908,9 @@
         <v>0.76</v>
       </c>
       <c r="F16">
-        <v>0.39</v>
+        <v>0.33</v>
       </c>
       <c r="G16">
-        <v>0.33</v>
-      </c>
-      <c r="H16">
         <v>0.8100000000000001</v>
       </c>
     </row>
@@ -2053,12 +1935,9 @@
         <v>0.59</v>
       </c>
       <c r="F17">
-        <v>0.55</v>
+        <v>0.82</v>
       </c>
       <c r="G17">
-        <v>0.82</v>
-      </c>
-      <c r="H17">
         <v>0.79</v>
       </c>
     </row>
@@ -2083,12 +1962,9 @@
         <v>0.65</v>
       </c>
       <c r="F18">
-        <v>0.54</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="G18">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="H18">
         <v>0.62</v>
       </c>
     </row>
@@ -2113,12 +1989,9 @@
         <v>0.65</v>
       </c>
       <c r="F19">
-        <v>0.49</v>
+        <v>0.48</v>
       </c>
       <c r="G19">
-        <v>0.48</v>
-      </c>
-      <c r="H19">
         <v>0.68</v>
       </c>
     </row>
@@ -2143,12 +2016,9 @@
         <v>0.31</v>
       </c>
       <c r="F20">
-        <v>0.76</v>
+        <v>0.79</v>
       </c>
       <c r="G20">
-        <v>0.79</v>
-      </c>
-      <c r="H20">
         <v>0.9</v>
       </c>
     </row>
@@ -2173,12 +2043,9 @@
         <v>0.77</v>
       </c>
       <c r="F21">
-        <v>0.4</v>
+        <v>0.48</v>
       </c>
       <c r="G21">
-        <v>0.48</v>
-      </c>
-      <c r="H21">
         <v>0.6899999999999999</v>
       </c>
     </row>
@@ -2203,12 +2070,9 @@
         <v>0.8100000000000001</v>
       </c>
       <c r="F22">
-        <v>0.42</v>
+        <v>0.3</v>
       </c>
       <c r="G22">
-        <v>0.3</v>
-      </c>
-      <c r="H22">
         <v>0.74</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Feedback, October 2023, markdown and figures
</commit_message>
<xml_diff>
--- a/paper/supplementary_tables.xlsx
+++ b/paper/supplementary_tables.xlsx
@@ -20,6 +20,7 @@
     <sheet name="Supplementary Table S10" sheetId="11" r:id="rId11"/>
     <sheet name="Supplementary Table S11" sheetId="12" r:id="rId12"/>
     <sheet name="Supplementary Table S12" sheetId="13" r:id="rId13"/>
+    <sheet name="Supplementary Table S13" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -363,7 +364,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -473,7 +474,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Significant differences in demographic, socioeconomic, clinical, accident- and recovery-related factors, and mental disorder symptoms between the mental clusters in the entire cohort. Numeric variables are presented as medians with interquartile ranges (IQR). Categorical variables are presented as percentages and counts within the complete observation set.</t>
+          <t>Frequency of mental disorder symptoms in the mental health clusters in the entire cohort. Categorical variables are presented as percentages and counts within the clusters.</t>
         </is>
       </c>
     </row>
@@ -485,7 +486,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Sets of explanatory factors used for modeling of the mental cluster assignment.</t>
+          <t>Differences in demographic, socioeconomic, clinical, accident- and recovery-related factors, and between the mental clusters in the entire cohort. Significant effects are presented, the full table is available as a supplementary Excel file. Numeric variables are presented as medians with interquartile ranges (IQR). Categorical variables are presented as percentages and counts within the clusters.</t>
         </is>
       </c>
     </row>
@@ -497,7 +498,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>The optimal combinations of machine learning algorithm parameters found in 10-fold cross-validation of the training subset of the study cohort.</t>
+          <t>Sets of explanatory factors used for modeling of the mental cluster assignment.</t>
         </is>
       </c>
     </row>
@@ -509,7 +510,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Performance statistics of machine learning classifiers at predicting the mental cluster assignment. Models employing early predictors available during acute medical management of the accident.</t>
+          <t>The optimal combinations of machine learning algorithm parameters found in 10-fold cross-validation of the training subset of the study cohort.</t>
         </is>
       </c>
     </row>
@@ -521,7 +522,19 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Performance statistics of machine learning classifiers at predicting the mental cluster assignment. Models employing the full predictor set available during acute medical management of the accident and follow-up.</t>
+          <t>Performance statistics of machine learning classifiers at predicting the mental cluster assignment. Models employing early predictors available during acute medical management of the patient.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Supplementary Table S13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Performance statistics of machine learning classifiers at predicting the mental cluster assignment. Models employing the full predictor set available during acute medical management of the patient and follow-up.</t>
         </is>
       </c>
     </row>
@@ -531,6 +544,1762 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Variable</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Neutral cluster</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>PTG cluster</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>PTS cluster</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Significance</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Effect size</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Participants, n</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>103</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>age at the accident, years</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>53 [IQR: 34 - 61]
+range: 18 - 82</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>54 [IQR: 39 - 61]
+range: 18 - 81</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>45 [IQR: 29 - 56]
+range: 18 - 82</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>p = 0.023</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>η² = 0.027</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>age at the accident, class, years</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>16-30: 19% (n = 20)
+31-65: 62% (n = 64)
+&gt;65: 18% (n = 19)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>16-30: 12% (n = 11)
+31-65: 74% (n = 70)
+&gt;65: 14% (n = 13)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>16-30: 27% (n = 30)
+31-65: 62% (n = 68)
+&gt;65: 11% (n = 12)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>ns (p = 0.11)</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>V = 0.13</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>hospital visit – survey time, days</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1400 [IQR: 760 - 1400]
+range: 400 - 1600</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1300 [IQR: 860 - 1400]
+range: 400 - 1500</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1300 [IQR: 960 - 1400]
+range: 390 - 1500</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>ns (p = 0.99)</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>η² = -0.0065</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>accident season</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>spring: 21% (n = 22)
+summer: 14% (n = 14)
+fall: 14% (n = 14)
+winter: 51% (n = 53)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>spring: 31% (n = 29)
+summer: 11% (n = 10)
+fall: 4.3% (n = 4)
+winter: 54% (n = 51)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>spring: 26% (n = 29)
+summer: 12% (n = 13)
+fall: 12% (n = 13)
+winter: 50% (n = 55)</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>ns (p = 0.47)</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>V = 0.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>accident daytime</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>day: 93% (n = 96)
+night: 6.8% (n = 7)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>day: 86% (n = 81)
+night: 14% (n = 13)</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>day: 93% (n = 102)
+night: 7.3% (n = 8)</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>ns (p = 0.27)</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>V = 0.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>sex</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>female: 36% (n = 37)
+male: 64% (n = 66)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>female: 50% (n = 47)
+male: 50% (n = 47)</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>female: 48% (n = 53)
+male: 52% (n = 57)</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>ns (p = 0.18)</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>V = 0.13</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>highest education grade</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>primary/apprenticeship: 9% (n = 9)
+secondary: 39% (n = 39)
+tertiary: 52% (n = 52)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>primary/apprenticeship: 26% (n = 24)
+secondary: 32% (n = 30)
+tertiary: 42% (n = 39)</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>primary/apprenticeship: 15% (n = 16)
+secondary: 43% (n = 46)
+tertiary: 42% (n = 45)</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>ns (p = 0.068)</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>V = 0.14</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>employment at the accident</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>employed: 69% (n = 71)
+unemployed: 2.9% (n = 3)
+student: 7.8% (n = 8)
+retired: 20% (n = 21)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>employed: 67% (n = 63)
+unemployed: 4.3% (n = 4)
+student: 7.4% (n = 7)
+retired: 21% (n = 20)</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>employed: 69% (n = 76)
+unemployed: 3.6% (n = 4)
+student: 15% (n = 17)
+retired: 12% (n = 13)</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>ns (p = 0.41)</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>V = 0.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>mountain sport profession</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>5.8% (n = 6)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>3.2% (n = 3)</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>6.4% (n = 7)</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>ns (p = 0.66)</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>V = 0.061</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>search and rescue profession</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>6.8% (n = 7)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>12% (n = 11)</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>3.6% (n = 4)</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>ns (p = 0.18)</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>V = 0.13</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>healthcare profession</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>4.9% (n = 5)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2.1% (n = 2)</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>1.8% (n = 2)</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>ns (p = 0.48)</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>V = 0.081</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>income/year</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>no income: 18% (n = 19)
+&lt; 30000 EUR: 16% (n = 16)
+30000 - 45000 EUR: 18% (n = 19)
+≥ 45000 EUR: 48% (n = 49)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>no income: 26% (n = 24)
+&lt; 30000 EUR: 20% (n = 19)
+30000 - 45000 EUR: 12% (n = 11)
+≥ 45000 EUR: 43% (n = 40)</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>no income: 18% (n = 20)
+&lt; 30000 EUR: 19% (n = 21)
+30000 - 45000 EUR: 26% (n = 29)
+≥ 45000 EUR: 36% (n = 40)</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>ns (p = 0.25)</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>V = 0.13</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>residence in the Alps</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>76% (n = 78)</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>70% (n = 66)</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>74% (n = 81)</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>ns (p = 0.75)</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>V = 0.05</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>smoking</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>9.7% (n = 10)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>4.3% (n = 4)</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>9.1% (n = 10)</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>ns (p = 0.45)</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>V = 0.089</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>pre-existing physical illness</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>5.8% (n = 6)</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>22% (n = 21)</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>18% (n = 20)</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>p = 0.013</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>V = 0.19</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>pre-existing physical illness type</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>none: 94% (n = 97)
+CVD: 1.9% (n = 2)
+neurological: 0% (n = 0)
+metabolic: 0% (n = 0)
+pulmonary: 0.97% (n = 1)
+cancer: 0% (n = 0)
+rheumatoid: 0% (n = 0)
+skin: 0% (n = 0)
+other: 2.9% (n = 3)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>none: 78% (n = 73)
+CVD: 5.3% (n = 5)
+neurological: 3.2% (n = 3)
+metabolic: 3.2% (n = 3)
+pulmonary: 0% (n = 0)
+cancer: 1.1% (n = 1)
+rheumatoid: 1.1% (n = 1)
+skin: 0% (n = 0)
+other: 8.5% (n = 8)</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>none: 82% (n = 90)
+CVD: 1.8% (n = 2)
+neurological: 0.91% (n = 1)
+metabolic: 0.91% (n = 1)
+pulmonary: 0.91% (n = 1)
+cancer: 0.91% (n = 1)
+rheumatoid: 0% (n = 0)
+skin: 0.91% (n = 1)
+other: 12% (n = 13)</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>ns (p = 0.18)</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>V = 0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>pre-existing diagnosed mental disorder</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>0% (n = 0)</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>1.1% (n = 1)</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>14% (n = 15)</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>V = 0.28</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>number of prior traumatic events/DIA-X</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>none: 70% (n = 72)
+1: 20% (n = 21)
+2: 7.8% (n = 8)
+3+: 1.9% (n = 2)</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>none: 51% (n = 48)
+1: 41% (n = 39)
+2: 4.3% (n = 4)
+3+: 3.2% (n = 3)</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>none: 57% (n = 63)
+1: 29% (n = 32)
+2: 10% (n = 11)
+3+: 3.6% (n = 4)</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>ns (p = 0.1)</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>V = 0.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>problematic alcohol use (CAGE ≥2)</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>7.8% (n = 8)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>7.4% (n = 7)</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>13% (n = 14)</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>ns (p = 0.47)</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>V = 0.084</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>prior mountain sport accidents</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>40% (n = 41)</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>35% (n = 33)</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>40% (n = 44)</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>ns (p = 0.77)</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>V = 0.046</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>accident year</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2018: 71% (n = 73)
+2019: 4.9% (n = 5)
+2020: 24% (n = 25)</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2018: 67% (n = 63)
+2019: 12% (n = 11)
+2020: 21% (n = 20)</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2018: 70% (n = 77)
+2019: 5.5% (n = 6)
+2020: 25% (n = 27)</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>ns (p = 0.48)</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>V = 0.084</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>mountain sport type</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ski/snowboard/cross-country: 62% (n = 64)
+sledding: 4.9% (n = 5)
+climbing/hiking/mountaineering/skitour: 12% (n = 12)
+biking: 20% (n = 21)
+other: 0.97% (n = 1)</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>ski/snowboard/cross-country: 70% (n = 66)
+sledding: 2.1% (n = 2)
+climbing/hiking/mountaineering/skitour: 13% (n = 12)
+biking: 13% (n = 12)
+other: 2.1% (n = 2)</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>ski/snowboard/cross-country: 61% (n = 67)
+sledding: 4.5% (n = 5)
+climbing/hiking/mountaineering/skitour: 16% (n = 18)
+biking: 14% (n = 15)
+other: 4.5% (n = 5)</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>ns (p = 0.56)</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>V = 0.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>alone during the accident</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>28% (n = 29)</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>39% (n = 37)</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>28% (n = 31)</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>ns (p = 0.26)</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>V = 0.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>responsible for the accident</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>self: 82% (n = 84)
+non-self: 18% (n = 19)</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>self: 67% (n = 63)
+non-self: 33% (n = 31)</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>self: 82% (n = 90)
+non-self: 18% (n = 20)</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>ns (p = 0.062)</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>V = 0.16</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>number of injured persons</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>only self: 65% (n = 67)
+self and partner: 5.8% (n = 6)
+3+ persons: 0.97% (n = 1)
+no information: 28% (n = 29)</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>only self: 56% (n = 53)
+self and partner: 3.2% (n = 3)
+3+ persons: 1.1% (n = 1)
+no information: 39% (n = 37)</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>only self: 68% (n = 75)
+self and partner: 1.8% (n = 2)
+3+ persons: 1.8% (n = 2)
+no information: 28% (n = 31)</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>ns (p = 0.48)</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>V = 0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>rescue mode</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>self: 61% (n = 63)
+companion: 19% (n = 20)
+rescue team: 19% (n = 20)</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>self: 43% (n = 40)
+companion: 21% (n = 20)
+rescue team: 36% (n = 34)</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>self: 47% (n = 52)
+companion: 21% (n = 23)
+rescue team: 32% (n = 35)</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>ns (p = 0.14)</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>V = 0.12</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>professional rescue mode</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>no professional rescue: 81% (n = 83)
+airborne: 8.7% (n = 9)
+on ground: 4.9% (n = 5)
+other: 5.8% (n = 6)</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>no professional rescue: 64% (n = 60)
+airborne: 17% (n = 16)
+on ground: 8.5% (n = 8)
+other: 11% (n = 10)</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>no professional rescue: 68% (n = 75)
+airborne: 14% (n = 15)
+on ground: 9.1% (n = 10)
+other: 9.1% (n = 10)</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>ns (p = 0.41)</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>V = 0.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>injury severity class, AIS</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>1: 44% (n = 42)
+2: 33% (n = 32)
+3+: 23% (n = 22)</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>1: 26% (n = 24)
+2: 41% (n = 38)
+3+: 33% (n = 30)</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>1: 40% (n = 42)
+2: 31% (n = 33)
+3+: 29% (n = 31)</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>ns (p = 0.21)</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>V = 0.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>injury severity, AIS</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2 [IQR: 1 - 2]
+range: 1 - 5</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2 [IQR: 1 - 3]
+range: 1 - 5</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2 [IQR: 1 - 3]
+range: 1 - 5</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>ns (p = 0.094)</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>η² = 0.016</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>head injury</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>12% (n = 12)</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>17% (n = 16)</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>14% (n = 15)</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>ns (p = 0.71)</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>V = 0.056</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>face injury</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>6.2% (n = 6)</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>14% (n = 13)</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>14% (n = 15)</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>ns (p = 0.25)</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>V = 0.12</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>neck injury</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>0% (n = 0)</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>1.1% (n = 1)</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>1.9% (n = 2)</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>ns (p = 0.52)</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>V = 0.078</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>chest injury</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>9.4% (n = 9)</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>11% (n = 10)</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>13% (n = 14)</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>ns (p = 0.75)</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>V = 0.051</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>abdomen injury</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>4.2% (n = 4)</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>4.3% (n = 4)</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>1.9% (n = 2)</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>ns (p = 0.66)</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>V = 0.063</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>spine region injury</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>9.4% (n = 9)</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>11% (n = 10)</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>9.4% (n = 10)</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>ns (p = 0.94)</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>V = 0.023</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>upper limb injury</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>42% (n = 40)</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>43% (n = 40)</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>38% (n = 40)</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>ns (p = 0.75)</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>V = 0.049</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>lower limb injury</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>40% (n = 38)</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>39% (n = 36)</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>50% (n = 53)</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>ns (p = 0.34)</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>V = 0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>other injury</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>16% (n = 15)</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>8.8% (n = 8)</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>14% (n = 15)</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>ns (p = 0.47)</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>V = 0.086</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>number of injured body parts</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>1 [IQR: 1 - 2]
+range: 1 - 4</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>1 [IQR: 1 - 2]
+range: 1 - 5</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>1 [IQR: 1 - 2]
+range: 1 - 7</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>ns (p = 0.66)</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>η² = -0.0027</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>hospitalized</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>17% (n = 17)</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>32% (n = 30)</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>30% (n = 33)</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>ns (p = 0.073)</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>V = 0.16</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>surgical therapy</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>7.8% (n = 8)</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>14% (n = 13)</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>20% (n = 22)</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>ns (p = 0.1)</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>V = 0.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>number of surgical ICD-10 diagnoses</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>none: 92% (n = 95)
+1: 5.8% (n = 6)
+2+: 1.9% (n = 2)</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>none: 86% (n = 81)
+1: 8.5% (n = 8)
+2+: 5.3% (n = 5)</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>none: 80% (n = 88)
+1: 11% (n = 12)
+2+: 9.1% (n = 10)</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>ns (p = 0.21)</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>V = 0.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>psychological/psychiatric support post accident</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>3.9% (n = 4)</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>13% (n = 12)</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>11% (n = 12)</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>ns (p = 0.15)</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>V = 0.13</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>psychological/psychiatric support need post accident</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>0% (n = 0)</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>8.5% (n = 8)</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>14% (n = 15)</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>p = 0.0039</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>V = 0.22</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>physical health consequences of the accident</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>27% (n = 28)</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>32% (n = 30)</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>52% (n = 57)</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>p = 0.0025</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>V = 0.23</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>returned to same mountain sport post accident</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>86% (n = 89)</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>87% (n = 82)</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>83% (n = 91)</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>ns (p = 0.71)</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>V = 0.056</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>caution during mountain sport post accident</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>no change: 50% (n = 52)
+more cautious: 49% (n = 50)
+less cautious: 0.97% (n = 1)</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>no change: 32% (n = 30)
+more cautious: 67% (n = 63)
+less cautious: 1.1% (n = 1)</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>no change: 22% (n = 24)
+more cautious: 78% (n = 86)
+less cautious: 0% (n = 0)</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>p = 0.0018</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>V = 0.19</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>confusion during mountain sport</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>4.9% (n = 5)</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>4.3% (n = 4)</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>3.6% (n = 4)</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>ns (p = 0.94)</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>V = 0.025</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -558,7 +2327,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>age, age class, accident season, accident daytime, sex, education, employment, sport profession, trauma-risk profession, healthcare profession, income/year, residence in the Alps, smoking, pre-existing physical illness, pre-existing physical illness type, pre-existing mental disorder, number of prior traumatic events/DIA-X, problematic alcohol use (CAGE ≥2), prior sport accidents, sport type, alone during the accident, responsible for the accident, injured persons, rescue, rescue mode, injury severity class, injury severity, head injury, face injury, neck injury, chest injury, abdomen injury, spine region injury, upper limb injury, lower limb injury, other injury, number of injured body parts, hospitalized, surgery, number of surgical ICD-10 diagnoses, psychological support, psychological support need, physical health consequences, returned to same sport, caution post accident, confusion during sport</t>
+          <t>age at the accident, age at the accident, class, accident season, accident daytime, sex, highest education grade, employment at the accident, mountain sport profession, search and rescue profession, healthcare profession, income/year, residence in the Alps, smoking, pre-existing physical illness, pre-existing physical illness type, pre-existing diagnosed mental disorder, number of prior traumatic events/DIA-X, problematic alcohol use (CAGE ≥2), prior mountain sport accidents, mountain sport type, alone during the accident, responsible for the accident, number of injured persons, rescue mode, professional rescue mode, injury severity class, injury severity, head injury, face injury, neck injury, chest injury, abdomen injury, spine region injury, upper limb injury, lower limb injury, other injury, number of injured body parts, hospitalized, surgical therapy, number of surgical ICD-10 diagnoses, psychological/psychiatric support post accident, psychological/psychiatric support need post accident, physical health consequences of the accident, returned to same mountain sport post accident, caution during mountain sport post accident, confusion during mountain sport</t>
         </is>
       </c>
     </row>
@@ -570,7 +2339,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>age, age class, accident season, accident daytime, sex, education, employment, sport profession, trauma-risk profession, healthcare profession, income/year, residence in the Alps, smoking, pre-existing physical illness, pre-existing physical illness type, pre-existing mental disorder, number of prior traumatic events/DIA-X, problematic alcohol use (CAGE ≥2), prior sport accidents, sport type, alone during the accident, responsible for the accident, injured persons, rescue, rescue mode, injury severity class, injury severity, head injury, face injury, neck injury, chest injury, abdomen injury, spine region injury, upper limb injury, lower limb injury, other injury, number of injured body parts, hospitalized, surgery, number of surgical ICD-10 diagnoses</t>
+          <t>age at the accident, age at the accident, class, accident season, accident daytime, sex, highest education grade, employment at the accident, mountain sport profession, search and rescue profession, healthcare profession, income/year, residence in the Alps, smoking, pre-existing physical illness, pre-existing physical illness type, pre-existing diagnosed mental disorder, number of prior traumatic events/DIA-X, problematic alcohol use (CAGE ≥2), prior mountain sport accidents, mountain sport type, alone during the accident, responsible for the accident, number of injured persons, rescue mode, professional rescue mode, injury severity class, injury severity, head injury, face injury, neck injury, chest injury, abdomen injury, spine region injury, upper limb injury, lower limb injury, other injury, number of injured body parts, hospitalized, surgical therapy, number of surgical ICD-10 diagnoses</t>
         </is>
       </c>
     </row>
@@ -579,7 +2348,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -840,623 +2609,6 @@
         <is>
           <t>alpha = 0.5, lambda = 0.0158</t>
         </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Algorithm</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Data subset</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Accuracy</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Cohen's κ</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Brier score</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Sensitivity, PTS cluster</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Specificity, PTS cluster</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>RF</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>training</t>
-        </is>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>0.99</v>
-      </c>
-      <c r="E2">
-        <v>0.15</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>RF</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>10-fold CV</t>
-        </is>
-      </c>
-      <c r="C3">
-        <v>0.41</v>
-      </c>
-      <c r="D3">
-        <v>0.11</v>
-      </c>
-      <c r="E3">
-        <v>0.68</v>
-      </c>
-      <c r="F3">
-        <v>0.42</v>
-      </c>
-      <c r="G3">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>RF</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="C4">
-        <v>0.47</v>
-      </c>
-      <c r="D4">
-        <v>0.21</v>
-      </c>
-      <c r="E4">
-        <v>0.66</v>
-      </c>
-      <c r="F4">
-        <v>0.48</v>
-      </c>
-      <c r="G4">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>NNet</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>training</t>
-        </is>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0.018</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>NNet</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>10-fold CV</t>
-        </is>
-      </c>
-      <c r="C6">
-        <v>0.45</v>
-      </c>
-      <c r="D6">
-        <v>0.17</v>
-      </c>
-      <c r="E6">
-        <v>0.88</v>
-      </c>
-      <c r="F6">
-        <v>0.35</v>
-      </c>
-      <c r="G6">
-        <v>0.6899999999999999</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>NNet</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="C7">
-        <v>0.38</v>
-      </c>
-      <c r="D7">
-        <v>0.078</v>
-      </c>
-      <c r="E7">
-        <v>0.96</v>
-      </c>
-      <c r="F7">
-        <v>0.33</v>
-      </c>
-      <c r="G7">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>SVM/radial</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>training</t>
-        </is>
-      </c>
-      <c r="C8">
-        <v>0.93</v>
-      </c>
-      <c r="D8">
-        <v>0.9</v>
-      </c>
-      <c r="E8">
-        <v>0.57</v>
-      </c>
-      <c r="F8">
-        <v>0.88</v>
-      </c>
-      <c r="G8">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>SVM/radial</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>10-fold CV</t>
-        </is>
-      </c>
-      <c r="C9">
-        <v>0.42</v>
-      </c>
-      <c r="D9">
-        <v>0.12</v>
-      </c>
-      <c r="E9">
-        <v>0.67</v>
-      </c>
-      <c r="F9">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="G9">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>SVM/radial</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="C10">
-        <v>0.47</v>
-      </c>
-      <c r="D10">
-        <v>0.21</v>
-      </c>
-      <c r="E10">
-        <v>0.66</v>
-      </c>
-      <c r="F10">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="G10">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>RPart</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>training</t>
-        </is>
-      </c>
-      <c r="C11">
-        <v>0.64</v>
-      </c>
-      <c r="D11">
-        <v>0.45</v>
-      </c>
-      <c r="E11">
-        <v>0.5</v>
-      </c>
-      <c r="F11">
-        <v>0.62</v>
-      </c>
-      <c r="G11">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>RPart</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>10-fold CV</t>
-        </is>
-      </c>
-      <c r="C12">
-        <v>0.38</v>
-      </c>
-      <c r="D12">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="E12">
-        <v>0.77</v>
-      </c>
-      <c r="F12">
-        <v>0.38</v>
-      </c>
-      <c r="G12">
-        <v>0.76</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>RPart</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="C13">
-        <v>0.34</v>
-      </c>
-      <c r="D13">
-        <v>0.018</v>
-      </c>
-      <c r="E13">
-        <v>0.78</v>
-      </c>
-      <c r="F13">
-        <v>0.33</v>
-      </c>
-      <c r="G13">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>SDA</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>training</t>
-        </is>
-      </c>
-      <c r="C14">
-        <v>0.68</v>
-      </c>
-      <c r="D14">
-        <v>0.52</v>
-      </c>
-      <c r="E14">
-        <v>0.41</v>
-      </c>
-      <c r="F14">
-        <v>0.68</v>
-      </c>
-      <c r="G14">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>SDA</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>10-fold CV</t>
-        </is>
-      </c>
-      <c r="C15">
-        <v>0.41</v>
-      </c>
-      <c r="D15">
-        <v>0.12</v>
-      </c>
-      <c r="E15">
-        <v>0.8</v>
-      </c>
-      <c r="F15">
-        <v>0.38</v>
-      </c>
-      <c r="G15">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>SDA</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="C16">
-        <v>0.39</v>
-      </c>
-      <c r="D16">
-        <v>0.094</v>
-      </c>
-      <c r="E16">
-        <v>0.74</v>
-      </c>
-      <c r="F16">
-        <v>0.33</v>
-      </c>
-      <c r="G16">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>cForest</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>training</t>
-        </is>
-      </c>
-      <c r="C17">
-        <v>0.7</v>
-      </c>
-      <c r="D17">
-        <v>0.55</v>
-      </c>
-      <c r="E17">
-        <v>0.55</v>
-      </c>
-      <c r="F17">
-        <v>0.75</v>
-      </c>
-      <c r="G17">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>cForest</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>10-fold CV</t>
-        </is>
-      </c>
-      <c r="C18">
-        <v>0.38</v>
-      </c>
-      <c r="D18">
-        <v>0.058</v>
-      </c>
-      <c r="E18">
-        <v>0.66</v>
-      </c>
-      <c r="F18">
-        <v>0.4</v>
-      </c>
-      <c r="G18">
-        <v>0.67</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>cForest</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="C19">
-        <v>0.46</v>
-      </c>
-      <c r="D19">
-        <v>0.2</v>
-      </c>
-      <c r="E19">
-        <v>0.65</v>
-      </c>
-      <c r="F19">
-        <v>0.48</v>
-      </c>
-      <c r="G19">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>ElasticNet</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>training</t>
-        </is>
-      </c>
-      <c r="C20">
-        <v>0.72</v>
-      </c>
-      <c r="D20">
-        <v>0.58</v>
-      </c>
-      <c r="E20">
-        <v>0.41</v>
-      </c>
-      <c r="F20">
-        <v>0.6899999999999999</v>
-      </c>
-      <c r="G20">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>ElasticNet</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>10-fold CV</t>
-        </is>
-      </c>
-      <c r="C21">
-        <v>0.42</v>
-      </c>
-      <c r="D21">
-        <v>0.13</v>
-      </c>
-      <c r="E21">
-        <v>0.76</v>
-      </c>
-      <c r="F21">
-        <v>0.38</v>
-      </c>
-      <c r="G21">
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>ElasticNet</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="C22">
-        <v>0.38</v>
-      </c>
-      <c r="D22">
-        <v>0.06900000000000001</v>
-      </c>
-      <c r="E22">
-        <v>0.74</v>
-      </c>
-      <c r="F22">
-        <v>0.41</v>
-      </c>
-      <c r="G22">
-        <v>0.62</v>
       </c>
     </row>
   </sheetData>
@@ -1521,6 +2673,623 @@
         </is>
       </c>
       <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0.99</v>
+      </c>
+      <c r="E2">
+        <v>0.15</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>10-fold CV</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>0.41</v>
+      </c>
+      <c r="D3">
+        <v>0.11</v>
+      </c>
+      <c r="E3">
+        <v>0.68</v>
+      </c>
+      <c r="F3">
+        <v>0.42</v>
+      </c>
+      <c r="G3">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>0.47</v>
+      </c>
+      <c r="D4">
+        <v>0.21</v>
+      </c>
+      <c r="E4">
+        <v>0.66</v>
+      </c>
+      <c r="F4">
+        <v>0.48</v>
+      </c>
+      <c r="G4">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>NNet</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>training</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0.018</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>NNet</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>10-fold CV</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>0.45</v>
+      </c>
+      <c r="D6">
+        <v>0.17</v>
+      </c>
+      <c r="E6">
+        <v>0.88</v>
+      </c>
+      <c r="F6">
+        <v>0.35</v>
+      </c>
+      <c r="G6">
+        <v>0.6899999999999999</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>NNet</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>0.38</v>
+      </c>
+      <c r="D7">
+        <v>0.078</v>
+      </c>
+      <c r="E7">
+        <v>0.96</v>
+      </c>
+      <c r="F7">
+        <v>0.33</v>
+      </c>
+      <c r="G7">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SVM/radial</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>training</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>0.93</v>
+      </c>
+      <c r="D8">
+        <v>0.9</v>
+      </c>
+      <c r="E8">
+        <v>0.57</v>
+      </c>
+      <c r="F8">
+        <v>0.88</v>
+      </c>
+      <c r="G8">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>SVM/radial</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>10-fold CV</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>0.42</v>
+      </c>
+      <c r="D9">
+        <v>0.12</v>
+      </c>
+      <c r="E9">
+        <v>0.67</v>
+      </c>
+      <c r="F9">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="G9">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>SVM/radial</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>0.47</v>
+      </c>
+      <c r="D10">
+        <v>0.21</v>
+      </c>
+      <c r="E10">
+        <v>0.66</v>
+      </c>
+      <c r="F10">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="G10">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>RPart</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>training</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>0.64</v>
+      </c>
+      <c r="D11">
+        <v>0.45</v>
+      </c>
+      <c r="E11">
+        <v>0.5</v>
+      </c>
+      <c r="F11">
+        <v>0.62</v>
+      </c>
+      <c r="G11">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>RPart</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>10-fold CV</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>0.38</v>
+      </c>
+      <c r="D12">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="E12">
+        <v>0.77</v>
+      </c>
+      <c r="F12">
+        <v>0.38</v>
+      </c>
+      <c r="G12">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>RPart</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C13">
+        <v>0.34</v>
+      </c>
+      <c r="D13">
+        <v>0.018</v>
+      </c>
+      <c r="E13">
+        <v>0.78</v>
+      </c>
+      <c r="F13">
+        <v>0.33</v>
+      </c>
+      <c r="G13">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>SDA</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>training</t>
+        </is>
+      </c>
+      <c r="C14">
+        <v>0.68</v>
+      </c>
+      <c r="D14">
+        <v>0.52</v>
+      </c>
+      <c r="E14">
+        <v>0.41</v>
+      </c>
+      <c r="F14">
+        <v>0.68</v>
+      </c>
+      <c r="G14">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>SDA</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>10-fold CV</t>
+        </is>
+      </c>
+      <c r="C15">
+        <v>0.41</v>
+      </c>
+      <c r="D15">
+        <v>0.12</v>
+      </c>
+      <c r="E15">
+        <v>0.8</v>
+      </c>
+      <c r="F15">
+        <v>0.38</v>
+      </c>
+      <c r="G15">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>SDA</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C16">
+        <v>0.39</v>
+      </c>
+      <c r="D16">
+        <v>0.094</v>
+      </c>
+      <c r="E16">
+        <v>0.74</v>
+      </c>
+      <c r="F16">
+        <v>0.33</v>
+      </c>
+      <c r="G16">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>cForest</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>training</t>
+        </is>
+      </c>
+      <c r="C17">
+        <v>0.7</v>
+      </c>
+      <c r="D17">
+        <v>0.55</v>
+      </c>
+      <c r="E17">
+        <v>0.55</v>
+      </c>
+      <c r="F17">
+        <v>0.75</v>
+      </c>
+      <c r="G17">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>cForest</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>10-fold CV</t>
+        </is>
+      </c>
+      <c r="C18">
+        <v>0.38</v>
+      </c>
+      <c r="D18">
+        <v>0.058</v>
+      </c>
+      <c r="E18">
+        <v>0.66</v>
+      </c>
+      <c r="F18">
+        <v>0.4</v>
+      </c>
+      <c r="G18">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>cForest</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C19">
+        <v>0.46</v>
+      </c>
+      <c r="D19">
+        <v>0.2</v>
+      </c>
+      <c r="E19">
+        <v>0.65</v>
+      </c>
+      <c r="F19">
+        <v>0.48</v>
+      </c>
+      <c r="G19">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>ElasticNet</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>training</t>
+        </is>
+      </c>
+      <c r="C20">
+        <v>0.72</v>
+      </c>
+      <c r="D20">
+        <v>0.58</v>
+      </c>
+      <c r="E20">
+        <v>0.41</v>
+      </c>
+      <c r="F20">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="G20">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>ElasticNet</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>10-fold CV</t>
+        </is>
+      </c>
+      <c r="C21">
+        <v>0.42</v>
+      </c>
+      <c r="D21">
+        <v>0.13</v>
+      </c>
+      <c r="E21">
+        <v>0.76</v>
+      </c>
+      <c r="F21">
+        <v>0.38</v>
+      </c>
+      <c r="G21">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>ElasticNet</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C22">
+        <v>0.38</v>
+      </c>
+      <c r="D22">
+        <v>0.06900000000000001</v>
+      </c>
+      <c r="E22">
+        <v>0.74</v>
+      </c>
+      <c r="F22">
+        <v>0.41</v>
+      </c>
+      <c r="G22">
+        <v>0.62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Algorithm</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Data subset</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Cohen's κ</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Brier score</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Sensitivity, PTS cluster</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Specificity, PTS cluster</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>training</t>
+        </is>
+      </c>
+      <c r="C2">
         <v>0.92</v>
       </c>
       <c r="D2">
@@ -2129,7 +3898,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>age</t>
+          <t>age at the accident</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2156,7 +3925,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>age class</t>
+          <t>age at the accident, class</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2296,7 +4065,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>highest education grade</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -2323,7 +4092,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>employment</t>
+          <t>employment at the accident</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -2350,12 +4119,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>sport profession</t>
+          <t>mountain sport profession</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Sport-related profession</t>
+          <t>Mountain sport-related profession</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -2377,12 +4146,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>trauma-risk profession</t>
+          <t>search and rescue profession</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Trauma-risk profession</t>
+          <t>Search and rescue service profession</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -2566,12 +4335,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>pre-existing mental disorder</t>
+          <t>pre-existing diagnosed mental disorder</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Mental disorder prior to the accident</t>
+          <t>Professionally diagnosed mental disorder prior to the accident</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -2647,12 +4416,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>prior sport accidents</t>
+          <t>prior mountain sport accidents</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Prior sport accidents</t>
+          <t>Prior mountain sport accidents</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -2701,12 +4470,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>sport type</t>
+          <t>mountain sport type</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Type of sport at the accident</t>
+          <t>Type of mountain sport at the accident</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -2782,12 +4551,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>injured persons</t>
+          <t>number of injured persons</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Accident injured persons</t>
+          <t>Number of injured persons during the mountain sport accident</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2809,12 +4578,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>rescue</t>
+          <t>rescue mode</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Accident rescue</t>
+          <t>Mode of accident rescue</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2824,7 +4593,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>self, partner/third party, rescue team</t>
+          <t>self, companion, rescue team</t>
         </is>
       </c>
     </row>
@@ -2836,12 +4605,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>rescue mode</t>
+          <t>professional rescue mode</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Accident rescue mode</t>
+          <t>Mode of professional accident rescue</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -3214,12 +4983,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>surgery</t>
+          <t>surgical therapy</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Need for surgical therapy</t>
+          <t>Surgical therapy of the accident’s injuries</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -3268,7 +5037,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>psychological support</t>
+          <t>psychological/psychiatric support post accident</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -3295,12 +5064,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>psychological support need</t>
+          <t>psychological/psychiatric support need post accident</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Subjective need for psychological support</t>
+          <t>Subjective need for psychological support after the accident</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3322,12 +5091,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>physical health consequences</t>
+          <t>physical health consequences of the accident</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Accident consequences felt, physical health health</t>
+          <t>Physical health consequences related to the accident</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3349,12 +5118,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>returned to same sport</t>
+          <t>returned to same mountain sport post accident</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Returned to the same sport activity post accident</t>
+          <t>Returned to the same mountain sport activity following the accident</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3376,12 +5145,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>caution post accident</t>
+          <t>caution during mountain sport post accident</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Caution after accident</t>
+          <t>Caution during mountain sport activity after the accident</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -3403,12 +5172,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>flashbacks during sport</t>
+          <t>flashbacks during mountain sport</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Flashback during sport activity</t>
+          <t>Flashback during mountain sport activity</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -3430,12 +5199,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>flashback frequency</t>
+          <t>flashback frequency during mountain sport</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Flashback frequency</t>
+          <t>Frequency of flashbacks during mountain sport activity</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -3457,12 +5226,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>confusion during sport</t>
+          <t>confusion during mountain sport</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Confusion during sport activity</t>
+          <t>Confusion during mountain sport activity after the accident</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -3506,7 +5275,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>PTSD+ (at least one PCL-5 domain)</t>
+          <t>PTSD symptoms (at least one PCL-5 domain positive)</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -3954,12 +5723,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Depression symptoms (PHQ-9 ≥11)</t>
+          <t>clinically relevant depression symptoms (PHQ-9 ≥11)</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>PHQ-9 score, depression symptoms</t>
+          <t>PHQ-9 score ≥ 11 points, clinically relevant depressive symptoms</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -4003,12 +5772,12 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Anxiety symptoms (GAD-7 ≥10)</t>
+          <t>clinically relevant anxiety symptoms (GAD-7 ≥10)</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>GAD-7 score, anxiety symptoms</t>
+          <t>GAD-7 score ≥ 10 points, clinically relevant anxiety symptoms</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -4052,7 +5821,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Panic symptoms (PHQ-panic)</t>
+          <t>clinically relevant panic symptoms (PHQ-panic)</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -4101,12 +5870,12 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Somatic symptoms (PHQ-15 ≥11)</t>
+          <t>clinically relevant somatizaton symptoms (PHQ-15 ≥11)</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>PHQ-15 health problems, clinically relevant somatic symptoms</t>
+          <t>PHQ-15 score ≥ 11 points, clinically relevant somatization symptoms</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -4373,7 +6142,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>PTSD+ (at least one PCL-5 domain)</t>
+          <t>PTSD symptoms (at least one PCL-5 domain positive)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -4696,12 +6465,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Depression symptoms (PHQ-9 ≥11)</t>
+          <t>clinically relevant depression symptoms (PHQ-9 ≥11)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>PHQ-9 score, depression symptoms</t>
+          <t>PHQ-9 score ≥ 11 points, clinically relevant depressive symptoms</t>
         </is>
       </c>
     </row>
@@ -4730,12 +6499,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Anxiety symptoms (GAD-7 ≥10)</t>
+          <t>clinically relevant anxiety symptoms (GAD-7 ≥10)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>GAD-7 score, anxiety symptoms</t>
+          <t>GAD-7 score ≥ 10 points, clinically relevant anxiety symptoms</t>
         </is>
       </c>
     </row>
@@ -4764,7 +6533,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Panic symptoms (PHQ-panic)</t>
+          <t>clinically relevant panic symptoms (PHQ-panic)</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -4798,12 +6567,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Somatic symptoms (PHQ-15 ≥11)</t>
+          <t>clinically relevant somatizaton symptoms (PHQ-15 ≥11)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>PHQ-15 health problems, clinically relevant somatic symptoms</t>
+          <t>PHQ-15 score ≥ 11 points, clinically relevant somatization symptoms</t>
         </is>
       </c>
     </row>
@@ -5150,7 +6919,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>sport type</t>
+          <t>mountain sport type</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -5282,7 +7051,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>surgery</t>
+          <t>surgical therapy</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -5508,7 +7277,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>surgery</t>
+          <t>surgical therapy</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -5537,7 +7306,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>physical health consequences</t>
+          <t>physical health consequences of the accident</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -7889,7 +9658,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7952,563 +9721,394 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>age, years</t>
+          <t>PTSD symptoms (at least one PCL-5 domain positive)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>53 [IQR: 34 - 61]
-range: 18 - 82</t>
+          <t>4.9% (n = 5)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>54 [IQR: 39 - 61]
-range: 18 - 81</t>
+          <t>15% (n = 14)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>45 [IQR: 29 - 56]
-range: 18 - 82</t>
+          <t>35% (n = 39)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>p = 0.023</t>
+          <t>p &lt; 0.001</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>η² = 0.027</t>
+          <t>V = 0.33</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>pre-existing physical illness</t>
+          <t>PTSD domain B symptoms</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5.8% (n = 6)</t>
+          <t>1.9% (n = 2)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>22% (n = 21)</t>
+          <t>9.6% (n = 9)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>18% (n = 20)</t>
+          <t>20% (n = 22)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>p = 0.013</t>
+          <t>p &lt; 0.001</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>V = 0.19</t>
+          <t>V = 0.24</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>pre-existing mental disorder</t>
+          <t>PTSD domain C symptoms</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0% (n = 0)</t>
+          <t>2.9% (n = 3)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.1% (n = 1)</t>
+          <t>5.3% (n = 5)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>14% (n = 15)</t>
+          <t>15% (n = 17)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>p &lt; 0.001</t>
+          <t>p = 0.0083</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>V = 0.28</t>
+          <t>V = 0.2</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>psychological support need</t>
+          <t>PTSD domain D symptoms</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0% (n = 0)</t>
+          <t>0.97% (n = 1)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>8.5% (n = 8)</t>
+          <t>3.2% (n = 3)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>14% (n = 15)</t>
+          <t>11% (n = 12)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>p = 0.0039</t>
+          <t>p = 0.012</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>V = 0.22</t>
+          <t>V = 0.2</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>physical health consequences</t>
+          <t>PTSD domain E symptoms</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>27% (n = 28)</t>
+          <t>0% (n = 0)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>32% (n = 30)</t>
+          <t>5.3% (n = 5)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>52% (n = 57)</t>
+          <t>17% (n = 19)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>p = 0.0025</t>
+          <t>p &lt; 0.001</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>V = 0.23</t>
+          <t>V = 0.27</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>caution post accident</t>
+          <t>flashbacks during mountain sport</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>no change: 50% (n = 52)
-more cautious: 49% (n = 50)
-less cautious: 0.97% (n = 1)</t>
+          <t>24% (n = 25)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>no change: 32% (n = 30)
-more cautious: 67% (n = 63)
-less cautious: 1.1% (n = 1)</t>
+          <t>35% (n = 33)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>no change: 22% (n = 24)
-more cautious: 78% (n = 86)
-less cautious: 0% (n = 0)</t>
+          <t>58% (n = 64)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>p = 0.0018</t>
+          <t>p &lt; 0.001</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>V = 0.19</t>
+          <t>V = 0.3</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>flashbacks during sport</t>
+          <t>flashback frequency during mountain sport</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
-        <is>
-          <t>24% (n = 25)</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>35% (n = 33)</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>58% (n = 64)</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>p &lt; 0.001</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>V = 0.3</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>flashback frequency</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
         <is>
           <t>none: 76% (n = 78)
 &gt; 1/year: 17% (n = 18)
 &gt; 1/month: 6.8% (n = 7)</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>none: 65% (n = 61)
 &gt; 1/year: 20% (n = 19)
 &gt; 1/month: 15% (n = 14)</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>none: 42% (n = 46)
 &gt; 1/year: 28% (n = 31)
 &gt; 1/month: 30% (n = 33)</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>p &lt; 0.001</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>V = 0.22</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>PTSD+ (at least one PCL-5 domain)</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>4.9% (n = 5)</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>15% (n = 14)</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>35% (n = 39)</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>p &lt; 0.001</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>V = 0.33</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>PTSD domain B symptoms</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1.9% (n = 2)</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>9.6% (n = 9)</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>20% (n = 22)</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>p &lt; 0.001</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>V = 0.24</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>PTSD domain C symptoms</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2.9% (n = 3)</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>5.3% (n = 5)</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>15% (n = 17)</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>p = 0.0083</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>V = 0.2</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>PTSD domain D symptoms</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>0.97% (n = 1)</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>3.2% (n = 3)</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>11% (n = 12)</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>p = 0.012</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>V = 0.2</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>PTSD domain E symptoms</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>0% (n = 0)</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>5.3% (n = 5)</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>17% (n = 19)</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>p &lt; 0.001</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>V = 0.27</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
+    <row r="10">
+      <c r="A10" t="inlineStr">
         <is>
           <t>RS13 resilience class</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>low: 3.9% (n = 4)
 moderate: 5.8% (n = 6)
 high: 90% (n = 93)</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>low: 6.4% (n = 6)
 moderate: 5.3% (n = 5)
 high: 88% (n = 83)</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>low: 42% (n = 46)
 moderate: 28% (n = 31)
 high: 30% (n = 33)</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>p &lt; 0.001</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>V = 0.43</t>
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Depression symptoms (PHQ-9 ≥11)</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>clinically relevant depression symptoms (PHQ-9 ≥11)</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>0% (n = 0)</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>2.1% (n = 2)</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>14% (n = 15)</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>p &lt; 0.001</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>V = 0.27</t>
         </is>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Anxiety symptoms (GAD-7 ≥10)</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>clinically relevant anxiety symptoms (GAD-7 ≥10)</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>0% (n = 0)</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>0% (n = 0)</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>6.4% (n = 7)</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>p = 0.0082</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>V = 0.2</t>
         </is>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Somatic symptoms (PHQ-15 ≥11)</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>clinically relevant panic symptoms (PHQ-panic)</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>0% (n = 0)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0% (n = 0)</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2.7% (n = 3)</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>ns (p = 0.15)</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>V = 0.13</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>clinically relevant somatizaton symptoms (PHQ-15 ≥11)</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>0.97% (n = 1)</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>3.2% (n = 3)</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>10% (n = 11)</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>p = 0.023</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>V = 0.18</t>
         </is>

</xml_diff>

<commit_message>
P2P reply, supplementary material
Changes in supplementary figures and tables required by the reviewer's comments
</commit_message>
<xml_diff>
--- a/paper/supplementary_tables.xlsx
+++ b/paper/supplementary_tables.xlsx
@@ -21,6 +21,7 @@
     <sheet name="Supplementary Table S11" sheetId="12" r:id="rId12"/>
     <sheet name="Supplementary Table S12" sheetId="13" r:id="rId13"/>
     <sheet name="Supplementary Table S13" sheetId="14" r:id="rId14"/>
+    <sheet name="Supplementary Table S14" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -364,7 +365,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -450,7 +451,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Significant differences between the training and test subset of the study cohort. Numeric variables are presented as medians with interquartile ranges (IQR). Categorical variables are presented as percentages and counts within the complete observation set.</t>
+          <t>Comparison of sociodemographic features of the study cohort and estimates for the general Austrian population. Numeric variables are presented as medians with interquartile ranges (IQR). Categorical variables are presented as percentages and counts within the complete observation set.</t>
         </is>
       </c>
     </row>
@@ -462,7 +463,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Differences in psychometric clustering factors between the mental clusters. Numeric variables are presented as medians with interquartile ranges (IQR). Statistical significance was determined by false discovery rate-corrected Kruskal-Wallis test with eta-square effect size statistic. The table is available in a supplementary Excel file.</t>
+          <t>Significant differences between the training and test subset of the study cohort. Numeric variables are presented as medians with interquartile ranges (IQR). Categorical variables are presented as percentages and counts within the complete observation set.</t>
         </is>
       </c>
     </row>
@@ -474,7 +475,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Frequency of mental disorder symptoms in the mental health clusters in the entire cohort. Categorical variables are presented as percentages and counts within the clusters.</t>
+          <t>Differences in psychometric clustering factors between the mental clusters. Numeric variables are presented as medians with interquartile ranges (IQR). Statistical significance was determined by false discovery rate-corrected Kruskal-Wallis test with eta-square effect size statistic. The table is available in a supplementary Excel file.</t>
         </is>
       </c>
     </row>
@@ -486,7 +487,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Differences in demographic, socioeconomic, clinical, accident- and recovery-related factors, and between the mental clusters in the entire cohort. Significant effects are presented, the full table is available as a supplementary Excel file. Numeric variables are presented as medians with interquartile ranges (IQR). Categorical variables are presented as percentages and counts within the clusters.</t>
+          <t>Frequency of mental disorder symptoms in the mental health clusters in the entire cohort. Categorical variables are presented as percentages and counts within the clusters.</t>
         </is>
       </c>
     </row>
@@ -498,7 +499,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Sets of explanatory factors used for modeling of the mental cluster assignment.</t>
+          <t>Differences in demographic, socioeconomic, clinical, accident- and recovery-related factors, and between the mental clusters in the entire cohort. Significant effects are presented, the full table is available as a supplementary Excel file. Numeric variables are presented as medians with interquartile ranges (IQR). Categorical variables are presented as percentages and counts within the clusters.</t>
         </is>
       </c>
     </row>
@@ -510,7 +511,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>The optimal combinations of machine learning algorithm parameters found in 10-fold cross-validation of the training subset of the study cohort.</t>
+          <t>Sets of explanatory factors used for modeling of the mental cluster assignment.</t>
         </is>
       </c>
     </row>
@@ -522,7 +523,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Performance statistics of machine learning classifiers at predicting the mental cluster assignment. Models employing early predictors available during acute medical management of the patient.</t>
+          <t>The optimal combinations of machine learning algorithm parameters found in 10-fold cross-validation of the training subset of the study cohort.</t>
         </is>
       </c>
     </row>
@@ -533,6 +534,18 @@
         </is>
       </c>
       <c r="B14" t="inlineStr">
+        <is>
+          <t>Performance statistics of machine learning classifiers at predicting the mental cluster assignment. Models employing early predictors available during acute medical management of the patient.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Supplementary Table S14</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>Performance statistics of machine learning classifiers at predicting the mental cluster assignment. Models employing the full predictor set available during acute medical management of the patient and follow-up.</t>
         </is>
@@ -544,6 +557,469 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Variable</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Neutral cluster</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>PTG cluster</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>PTS cluster</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Significance</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Effect size</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Participants, n</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>103</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>PTSD symptoms (at least one PCL-5 domain positive)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>4.9% (n = 5)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>15% (n = 14)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>35% (n = 39)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>V = 0.33</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>PTSD domain B symptoms</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1.9% (n = 2)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>9.6% (n = 9)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>20% (n = 22)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>V = 0.24</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>PTSD domain C symptoms</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2.9% (n = 3)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>5.3% (n = 5)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>15% (n = 17)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>p = 0.0083</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>V = 0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>PTSD domain D symptoms</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0.97% (n = 1)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>3.2% (n = 3)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>11% (n = 12)</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>p = 0.012</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>V = 0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>PTSD domain E symptoms</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0% (n = 0)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>5.3% (n = 5)</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>17% (n = 19)</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>V = 0.27</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>flashbacks during mountain sport</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>24% (n = 25)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>35% (n = 33)</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>58% (n = 64)</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>V = 0.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>flashback frequency during mountain sport</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>none: 76% (n = 78)
+&gt; 1/year: 17% (n = 18)
+&gt; 1/month: 6.8% (n = 7)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>none: 65% (n = 61)
+&gt; 1/year: 20% (n = 19)
+&gt; 1/month: 15% (n = 14)</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>none: 42% (n = 46)
+&gt; 1/year: 28% (n = 31)
+&gt; 1/month: 30% (n = 33)</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>V = 0.22</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>RS13 resilience class</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>low: 3.9% (n = 4)
+moderate: 5.8% (n = 6)
+high: 90% (n = 93)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>low: 6.4% (n = 6)
+moderate: 5.3% (n = 5)
+high: 88% (n = 83)</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>low: 42% (n = 46)
+moderate: 28% (n = 31)
+high: 30% (n = 33)</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>V = 0.43</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>clinically relevant depression symptoms (PHQ-9 ≥11)</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>0% (n = 0)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2.1% (n = 2)</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>14% (n = 15)</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>V = 0.27</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>clinically relevant anxiety symptoms (GAD-7 ≥10)</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>0% (n = 0)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0% (n = 0)</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>6.4% (n = 7)</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>p = 0.0082</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>V = 0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>clinically relevant panic symptoms (PHQ-panic)</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>0% (n = 0)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0% (n = 0)</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2.7% (n = 3)</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>ns (p = 0.15)</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>V = 0.13</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>clinically relevant somatizaton symptoms (PHQ-15 ≥11)</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>0.97% (n = 1)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>3.2% (n = 3)</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>10% (n = 11)</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>p = 0.023</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>V = 0.18</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F50"/>
   <sheetViews>
@@ -648,21 +1124,21 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16-30: 19% (n = 20)
+          <t>18-30: 19% (n = 20)
 31-65: 62% (n = 64)
 &gt;65: 18% (n = 19)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>16-30: 12% (n = 11)
+          <t>18-30: 12% (n = 11)
 31-65: 74% (n = 70)
 &gt;65: 14% (n = 13)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>16-30: 27% (n = 30)
+          <t>18-30: 27% (n = 30)
 31-65: 62% (n = 68)
 &gt;65: 11% (n = 12)</t>
         </is>
@@ -2299,7 +2775,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2348,7 +2824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -2609,623 +3085,6 @@
         <is>
           <t>alpha = 0.5, lambda = 0.0158</t>
         </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Algorithm</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Data subset</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Accuracy</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Cohen's κ</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Brier score</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Sensitivity, PTS cluster</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Specificity, PTS cluster</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>RF</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>training</t>
-        </is>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>0.99</v>
-      </c>
-      <c r="E2">
-        <v>0.15</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>RF</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>10-fold CV</t>
-        </is>
-      </c>
-      <c r="C3">
-        <v>0.41</v>
-      </c>
-      <c r="D3">
-        <v>0.11</v>
-      </c>
-      <c r="E3">
-        <v>0.68</v>
-      </c>
-      <c r="F3">
-        <v>0.42</v>
-      </c>
-      <c r="G3">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>RF</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="C4">
-        <v>0.47</v>
-      </c>
-      <c r="D4">
-        <v>0.21</v>
-      </c>
-      <c r="E4">
-        <v>0.66</v>
-      </c>
-      <c r="F4">
-        <v>0.48</v>
-      </c>
-      <c r="G4">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>NNet</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>training</t>
-        </is>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0.018</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>NNet</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>10-fold CV</t>
-        </is>
-      </c>
-      <c r="C6">
-        <v>0.45</v>
-      </c>
-      <c r="D6">
-        <v>0.17</v>
-      </c>
-      <c r="E6">
-        <v>0.88</v>
-      </c>
-      <c r="F6">
-        <v>0.35</v>
-      </c>
-      <c r="G6">
-        <v>0.6899999999999999</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>NNet</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="C7">
-        <v>0.38</v>
-      </c>
-      <c r="D7">
-        <v>0.078</v>
-      </c>
-      <c r="E7">
-        <v>0.96</v>
-      </c>
-      <c r="F7">
-        <v>0.33</v>
-      </c>
-      <c r="G7">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>SVM/radial</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>training</t>
-        </is>
-      </c>
-      <c r="C8">
-        <v>0.93</v>
-      </c>
-      <c r="D8">
-        <v>0.9</v>
-      </c>
-      <c r="E8">
-        <v>0.57</v>
-      </c>
-      <c r="F8">
-        <v>0.88</v>
-      </c>
-      <c r="G8">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>SVM/radial</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>10-fold CV</t>
-        </is>
-      </c>
-      <c r="C9">
-        <v>0.42</v>
-      </c>
-      <c r="D9">
-        <v>0.12</v>
-      </c>
-      <c r="E9">
-        <v>0.67</v>
-      </c>
-      <c r="F9">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="G9">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>SVM/radial</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="C10">
-        <v>0.47</v>
-      </c>
-      <c r="D10">
-        <v>0.21</v>
-      </c>
-      <c r="E10">
-        <v>0.66</v>
-      </c>
-      <c r="F10">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="G10">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>RPart</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>training</t>
-        </is>
-      </c>
-      <c r="C11">
-        <v>0.64</v>
-      </c>
-      <c r="D11">
-        <v>0.45</v>
-      </c>
-      <c r="E11">
-        <v>0.5</v>
-      </c>
-      <c r="F11">
-        <v>0.62</v>
-      </c>
-      <c r="G11">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>RPart</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>10-fold CV</t>
-        </is>
-      </c>
-      <c r="C12">
-        <v>0.38</v>
-      </c>
-      <c r="D12">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="E12">
-        <v>0.77</v>
-      </c>
-      <c r="F12">
-        <v>0.38</v>
-      </c>
-      <c r="G12">
-        <v>0.76</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>RPart</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="C13">
-        <v>0.34</v>
-      </c>
-      <c r="D13">
-        <v>0.018</v>
-      </c>
-      <c r="E13">
-        <v>0.78</v>
-      </c>
-      <c r="F13">
-        <v>0.33</v>
-      </c>
-      <c r="G13">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>SDA</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>training</t>
-        </is>
-      </c>
-      <c r="C14">
-        <v>0.68</v>
-      </c>
-      <c r="D14">
-        <v>0.52</v>
-      </c>
-      <c r="E14">
-        <v>0.41</v>
-      </c>
-      <c r="F14">
-        <v>0.68</v>
-      </c>
-      <c r="G14">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>SDA</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>10-fold CV</t>
-        </is>
-      </c>
-      <c r="C15">
-        <v>0.41</v>
-      </c>
-      <c r="D15">
-        <v>0.12</v>
-      </c>
-      <c r="E15">
-        <v>0.8</v>
-      </c>
-      <c r="F15">
-        <v>0.38</v>
-      </c>
-      <c r="G15">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>SDA</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="C16">
-        <v>0.39</v>
-      </c>
-      <c r="D16">
-        <v>0.094</v>
-      </c>
-      <c r="E16">
-        <v>0.74</v>
-      </c>
-      <c r="F16">
-        <v>0.33</v>
-      </c>
-      <c r="G16">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>cForest</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>training</t>
-        </is>
-      </c>
-      <c r="C17">
-        <v>0.7</v>
-      </c>
-      <c r="D17">
-        <v>0.55</v>
-      </c>
-      <c r="E17">
-        <v>0.55</v>
-      </c>
-      <c r="F17">
-        <v>0.75</v>
-      </c>
-      <c r="G17">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>cForest</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>10-fold CV</t>
-        </is>
-      </c>
-      <c r="C18">
-        <v>0.38</v>
-      </c>
-      <c r="D18">
-        <v>0.058</v>
-      </c>
-      <c r="E18">
-        <v>0.66</v>
-      </c>
-      <c r="F18">
-        <v>0.4</v>
-      </c>
-      <c r="G18">
-        <v>0.67</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>cForest</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="C19">
-        <v>0.46</v>
-      </c>
-      <c r="D19">
-        <v>0.2</v>
-      </c>
-      <c r="E19">
-        <v>0.65</v>
-      </c>
-      <c r="F19">
-        <v>0.48</v>
-      </c>
-      <c r="G19">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>ElasticNet</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>training</t>
-        </is>
-      </c>
-      <c r="C20">
-        <v>0.72</v>
-      </c>
-      <c r="D20">
-        <v>0.58</v>
-      </c>
-      <c r="E20">
-        <v>0.41</v>
-      </c>
-      <c r="F20">
-        <v>0.6899999999999999</v>
-      </c>
-      <c r="G20">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>ElasticNet</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>10-fold CV</t>
-        </is>
-      </c>
-      <c r="C21">
-        <v>0.42</v>
-      </c>
-      <c r="D21">
-        <v>0.13</v>
-      </c>
-      <c r="E21">
-        <v>0.76</v>
-      </c>
-      <c r="F21">
-        <v>0.38</v>
-      </c>
-      <c r="G21">
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>ElasticNet</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="C22">
-        <v>0.38</v>
-      </c>
-      <c r="D22">
-        <v>0.06900000000000001</v>
-      </c>
-      <c r="E22">
-        <v>0.74</v>
-      </c>
-      <c r="F22">
-        <v>0.41</v>
-      </c>
-      <c r="G22">
-        <v>0.62</v>
       </c>
     </row>
   </sheetData>
@@ -3290,6 +3149,623 @@
         </is>
       </c>
       <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0.99</v>
+      </c>
+      <c r="E2">
+        <v>0.15</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>10-fold CV</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>0.41</v>
+      </c>
+      <c r="D3">
+        <v>0.11</v>
+      </c>
+      <c r="E3">
+        <v>0.68</v>
+      </c>
+      <c r="F3">
+        <v>0.42</v>
+      </c>
+      <c r="G3">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>0.47</v>
+      </c>
+      <c r="D4">
+        <v>0.21</v>
+      </c>
+      <c r="E4">
+        <v>0.66</v>
+      </c>
+      <c r="F4">
+        <v>0.48</v>
+      </c>
+      <c r="G4">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>NNet</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>training</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0.018</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>NNet</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>10-fold CV</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>0.45</v>
+      </c>
+      <c r="D6">
+        <v>0.17</v>
+      </c>
+      <c r="E6">
+        <v>0.88</v>
+      </c>
+      <c r="F6">
+        <v>0.35</v>
+      </c>
+      <c r="G6">
+        <v>0.6899999999999999</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>NNet</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>0.38</v>
+      </c>
+      <c r="D7">
+        <v>0.078</v>
+      </c>
+      <c r="E7">
+        <v>0.96</v>
+      </c>
+      <c r="F7">
+        <v>0.33</v>
+      </c>
+      <c r="G7">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SVM/radial</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>training</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>0.93</v>
+      </c>
+      <c r="D8">
+        <v>0.9</v>
+      </c>
+      <c r="E8">
+        <v>0.57</v>
+      </c>
+      <c r="F8">
+        <v>0.88</v>
+      </c>
+      <c r="G8">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>SVM/radial</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>10-fold CV</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>0.42</v>
+      </c>
+      <c r="D9">
+        <v>0.12</v>
+      </c>
+      <c r="E9">
+        <v>0.67</v>
+      </c>
+      <c r="F9">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="G9">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>SVM/radial</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>0.47</v>
+      </c>
+      <c r="D10">
+        <v>0.21</v>
+      </c>
+      <c r="E10">
+        <v>0.66</v>
+      </c>
+      <c r="F10">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="G10">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>RPart</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>training</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>0.64</v>
+      </c>
+      <c r="D11">
+        <v>0.45</v>
+      </c>
+      <c r="E11">
+        <v>0.5</v>
+      </c>
+      <c r="F11">
+        <v>0.62</v>
+      </c>
+      <c r="G11">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>RPart</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>10-fold CV</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>0.38</v>
+      </c>
+      <c r="D12">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="E12">
+        <v>0.77</v>
+      </c>
+      <c r="F12">
+        <v>0.38</v>
+      </c>
+      <c r="G12">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>RPart</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C13">
+        <v>0.34</v>
+      </c>
+      <c r="D13">
+        <v>0.018</v>
+      </c>
+      <c r="E13">
+        <v>0.78</v>
+      </c>
+      <c r="F13">
+        <v>0.33</v>
+      </c>
+      <c r="G13">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>SDA</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>training</t>
+        </is>
+      </c>
+      <c r="C14">
+        <v>0.68</v>
+      </c>
+      <c r="D14">
+        <v>0.52</v>
+      </c>
+      <c r="E14">
+        <v>0.41</v>
+      </c>
+      <c r="F14">
+        <v>0.68</v>
+      </c>
+      <c r="G14">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>SDA</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>10-fold CV</t>
+        </is>
+      </c>
+      <c r="C15">
+        <v>0.41</v>
+      </c>
+      <c r="D15">
+        <v>0.12</v>
+      </c>
+      <c r="E15">
+        <v>0.8</v>
+      </c>
+      <c r="F15">
+        <v>0.38</v>
+      </c>
+      <c r="G15">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>SDA</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C16">
+        <v>0.39</v>
+      </c>
+      <c r="D16">
+        <v>0.094</v>
+      </c>
+      <c r="E16">
+        <v>0.74</v>
+      </c>
+      <c r="F16">
+        <v>0.33</v>
+      </c>
+      <c r="G16">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>cForest</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>training</t>
+        </is>
+      </c>
+      <c r="C17">
+        <v>0.7</v>
+      </c>
+      <c r="D17">
+        <v>0.55</v>
+      </c>
+      <c r="E17">
+        <v>0.55</v>
+      </c>
+      <c r="F17">
+        <v>0.75</v>
+      </c>
+      <c r="G17">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>cForest</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>10-fold CV</t>
+        </is>
+      </c>
+      <c r="C18">
+        <v>0.38</v>
+      </c>
+      <c r="D18">
+        <v>0.058</v>
+      </c>
+      <c r="E18">
+        <v>0.66</v>
+      </c>
+      <c r="F18">
+        <v>0.4</v>
+      </c>
+      <c r="G18">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>cForest</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C19">
+        <v>0.46</v>
+      </c>
+      <c r="D19">
+        <v>0.2</v>
+      </c>
+      <c r="E19">
+        <v>0.65</v>
+      </c>
+      <c r="F19">
+        <v>0.48</v>
+      </c>
+      <c r="G19">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>ElasticNet</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>training</t>
+        </is>
+      </c>
+      <c r="C20">
+        <v>0.72</v>
+      </c>
+      <c r="D20">
+        <v>0.58</v>
+      </c>
+      <c r="E20">
+        <v>0.41</v>
+      </c>
+      <c r="F20">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="G20">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>ElasticNet</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>10-fold CV</t>
+        </is>
+      </c>
+      <c r="C21">
+        <v>0.42</v>
+      </c>
+      <c r="D21">
+        <v>0.13</v>
+      </c>
+      <c r="E21">
+        <v>0.76</v>
+      </c>
+      <c r="F21">
+        <v>0.38</v>
+      </c>
+      <c r="G21">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>ElasticNet</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C22">
+        <v>0.38</v>
+      </c>
+      <c r="D22">
+        <v>0.06900000000000001</v>
+      </c>
+      <c r="E22">
+        <v>0.74</v>
+      </c>
+      <c r="F22">
+        <v>0.41</v>
+      </c>
+      <c r="G22">
+        <v>0.62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Algorithm</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Data subset</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Cohen's κ</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Brier score</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Sensitivity, PTS cluster</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Specificity, PTS cluster</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>training</t>
+        </is>
+      </c>
+      <c r="C2">
         <v>0.92</v>
       </c>
       <c r="D2">
@@ -3945,7 +4421,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>16-30, 31-65, &gt;65</t>
+          <t>18-30, 31-65, &gt;65</t>
         </is>
       </c>
     </row>
@@ -7339,6 +7815,267 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Variable</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Cohort</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Austrian population</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Significance</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Effect size</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>age, years</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>51 [IQR: 33 - 60]
+range: 18 - 82
+n = 307</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>48 [IQR: 34 - 62]
+range: 18 - 82
+n = 7196298</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ns (p = 0.99)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>r = 4.9e-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>age, class, years</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>18-30: 20% (n = 61)
+31-65: 66% (n = 202)
+&gt;65: 14% (n = 44)
+n = 307</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>18-30: 20% (n = 1404528)
+31-65: 62% (n = 4452200)
+&gt;65: 19% (n = 1339570)
+n = 7196298</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>ns (p = 0.15)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>V = 0.00073</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>sex</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>female: 45% (n = 137)
+male: 55% (n = 170)
+n = 307</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>female: 51% (n = 3643212)
+male: 49% (n = 3553086)
+n = 7196298</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>p = 0.041</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>V = 0.00078</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>highest education grade</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>primary/apprenticeship: 16% (n = 49)
+secondary: 38% (n = 115)
+tertiary: 45% (n = 136)
+n = 300</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>primary/apprenticeship: 50% (n = 2511913)
+secondary: 30% (n = 1472534)
+tertiary: 20% (n = 995515)
+n = 4979962</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>V = 0.0059</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>employment</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>employed: 68% (n = 210)
+unemployed: 3.6% (n = 11)
+student: 10% (n = 32)
+retired: 18% (n = 54)
+n = 307</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>employed: 58% (n = 4438154)
+unemployed: 12% (n = 921539)
+student: 4.4% (n = 336979)
+retired: 26% (n = 1980715)
+n = 7677387</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>V = 0.0027</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>smoking</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>7.8% (n = 24)
+n = 307</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>26% (n = 1943745)
+n = 7417876</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>V = 0.0027</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>physical or mental illness</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>20% (n = 60)
+n = 307</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>38% (n = 2841553)
+n = 7417876</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>V = 0.0025</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7472,7 +8209,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G55"/>
   <sheetViews>
@@ -9654,467 +10391,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Variable</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Neutral cluster</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>PTG cluster</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>PTS cluster</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Significance</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Effect size</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Participants, n</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>94</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>PTSD symptoms (at least one PCL-5 domain positive)</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>4.9% (n = 5)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>15% (n = 14)</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>35% (n = 39)</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>p &lt; 0.001</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>V = 0.33</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>PTSD domain B symptoms</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1.9% (n = 2)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>9.6% (n = 9)</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>20% (n = 22)</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>p &lt; 0.001</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>V = 0.24</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>PTSD domain C symptoms</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2.9% (n = 3)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>5.3% (n = 5)</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>15% (n = 17)</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>p = 0.0083</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>V = 0.2</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>PTSD domain D symptoms</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>0.97% (n = 1)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>3.2% (n = 3)</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>11% (n = 12)</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>p = 0.012</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>V = 0.2</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>PTSD domain E symptoms</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>0% (n = 0)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>5.3% (n = 5)</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>17% (n = 19)</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>p &lt; 0.001</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>V = 0.27</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>flashbacks during mountain sport</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>24% (n = 25)</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>35% (n = 33)</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>58% (n = 64)</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>p &lt; 0.001</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>V = 0.3</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>flashback frequency during mountain sport</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>none: 76% (n = 78)
-&gt; 1/year: 17% (n = 18)
-&gt; 1/month: 6.8% (n = 7)</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>none: 65% (n = 61)
-&gt; 1/year: 20% (n = 19)
-&gt; 1/month: 15% (n = 14)</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>none: 42% (n = 46)
-&gt; 1/year: 28% (n = 31)
-&gt; 1/month: 30% (n = 33)</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>p &lt; 0.001</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>V = 0.22</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>RS13 resilience class</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>low: 3.9% (n = 4)
-moderate: 5.8% (n = 6)
-high: 90% (n = 93)</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>low: 6.4% (n = 6)
-moderate: 5.3% (n = 5)
-high: 88% (n = 83)</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>low: 42% (n = 46)
-moderate: 28% (n = 31)
-high: 30% (n = 33)</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>p &lt; 0.001</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>V = 0.43</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>clinically relevant depression symptoms (PHQ-9 ≥11)</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>0% (n = 0)</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>2.1% (n = 2)</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>14% (n = 15)</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>p &lt; 0.001</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>V = 0.27</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>clinically relevant anxiety symptoms (GAD-7 ≥10)</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>0% (n = 0)</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>0% (n = 0)</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>6.4% (n = 7)</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>p = 0.0082</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>V = 0.2</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>clinically relevant panic symptoms (PHQ-panic)</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>0% (n = 0)</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>0% (n = 0)</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>2.7% (n = 3)</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>ns (p = 0.15)</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>V = 0.13</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>clinically relevant somatizaton symptoms (PHQ-15 ≥11)</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>0.97% (n = 1)</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>3.2% (n = 3)</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>10% (n = 11)</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>p = 0.023</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>V = 0.18</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Revised figures, tables, manuscript and supplement
</commit_message>
<xml_diff>
--- a/paper/supplementary_tables.xlsx
+++ b/paper/supplementary_tables.xlsx
@@ -889,7 +889,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>clinically relevant depression symptoms (PHQ-9 ≥11)</t>
+          <t>clinically relevant depression symptoms (PHQ-9 ≥10)</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -904,7 +904,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>14% (n = 15)</t>
+          <t>18% (n = 20)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -914,7 +914,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>V = 0.27</t>
+          <t>V = 0.32</t>
         </is>
       </c>
     </row>
@@ -936,17 +936,17 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>6.4% (n = 7)</t>
+          <t>8.2% (n = 9)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>p = 0.0082</t>
+          <t>p = 0.0016</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>V = 0.2</t>
+          <t>V = 0.23</t>
         </is>
       </c>
     </row>
@@ -1402,7 +1402,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>ns (p = 0.66)</t>
+          <t>ns (p = 0.68)</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1539,7 +1539,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>ns (p = 0.75)</t>
+          <t>ns (p = 0.76)</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1796,7 +1796,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>ns (p = 0.77)</t>
+          <t>ns (p = 0.78)</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1851,39 +1851,60 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ski/snowboard/cross-country: 62% (n = 64)
+          <t>alpine skiing/snowboarding: 55% (n = 57)
+ski touring/freeride: 1.9% (n = 2)
+cross-country skiing: 6.8% (n = 7)
 sledding: 4.9% (n = 5)
-climbing/hiking/mountaineering/skitour: 12% (n = 12)
+ice climbing: 0% (n = 0)
+hiking: 3.9% (n = 4)
+climbing: 2.9% (n = 3)
+mountaineering: 0.97% (n = 1)
 biking: 20% (n = 21)
+air sport: 0.97% (n = 1)
+water sport: 0.97% (n = 1)
 other: 0.97% (n = 1)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ski/snowboard/cross-country: 70% (n = 66)
+          <t>alpine skiing/snowboarding: 65% (n = 61)
+ski touring/freeride: 3.2% (n = 3)
+cross-country skiing: 5.3% (n = 5)
 sledding: 2.1% (n = 2)
-climbing/hiking/mountaineering/skitour: 13% (n = 12)
+ice climbing: 1.1% (n = 1)
+hiking: 6.4% (n = 6)
+climbing: 2.1% (n = 2)
+mountaineering: 0% (n = 0)
 biking: 13% (n = 12)
-other: 2.1% (n = 2)</t>
+air sport: 0% (n = 0)
+water sport: 1.1% (n = 1)
+other: 1.1% (n = 1)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>ski/snowboard/cross-country: 61% (n = 67)
+          <t>alpine skiing/snowboarding: 56% (n = 62)
+ski touring/freeride: 3.6% (n = 4)
+cross-country skiing: 4.5% (n = 5)
 sledding: 4.5% (n = 5)
-climbing/hiking/mountaineering/skitour: 16% (n = 18)
+ice climbing: 0% (n = 0)
+hiking: 6.4% (n = 7)
+climbing: 5.5% (n = 6)
+mountaineering: 0.91% (n = 1)
 biking: 14% (n = 15)
-other: 4.5% (n = 5)</t>
+air sport: 0% (n = 0)
+water sport: 2.7% (n = 3)
+other: 1.8% (n = 2)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>ns (p = 0.56)</t>
+          <t>ns (p = 0.92)</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>V = 0.11</t>
+          <t>V = 0.15</t>
         </is>
       </c>
     </row>
@@ -2170,7 +2191,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>ns (p = 0.71)</t>
+          <t>ns (p = 0.72)</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2266,7 +2287,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>ns (p = 0.75)</t>
+          <t>ns (p = 0.76)</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2298,7 +2319,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>ns (p = 0.66)</t>
+          <t>ns (p = 0.68)</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2362,7 +2383,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>ns (p = 0.75)</t>
+          <t>ns (p = 0.76)</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2461,7 +2482,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>ns (p = 0.66)</t>
+          <t>ns (p = 0.68)</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2627,7 +2648,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>p = 0.0039</t>
+          <t>p = 0.0036</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -2659,7 +2680,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>p = 0.0025</t>
+          <t>p = 0.0023</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -2691,7 +2712,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>ns (p = 0.71)</t>
+          <t>ns (p = 0.72)</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2729,7 +2750,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>p = 0.0018</t>
+          <t>p = 0.0016</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -2862,7 +2883,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>mtry = 2, splitrule = gini, min.node.size = 3</t>
+          <t>mtry = 37, splitrule = extratrees, min.node.size = 5</t>
         </is>
       </c>
     </row>
@@ -2879,7 +2900,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>size = 2, decay = 0.01</t>
+          <t>size = 6, decay = 1e-04</t>
         </is>
       </c>
     </row>
@@ -2896,7 +2917,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>sigma = 0.02, C = 1.3</t>
+          <t>sigma = 0.02, C = 3.7</t>
         </is>
       </c>
     </row>
@@ -2930,7 +2951,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>diagonal = FALSE, lambda = 0.195</t>
+          <t>diagonal = FALSE, lambda = 0.335</t>
         </is>
       </c>
     </row>
@@ -2947,7 +2968,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>mtry = 4</t>
+          <t>mtry = 7</t>
         </is>
       </c>
     </row>
@@ -2964,7 +2985,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>alpha = 0.5, lambda = 0.01</t>
+          <t>alpha = 0.5, lambda = 0.00395</t>
         </is>
       </c>
     </row>
@@ -2981,7 +3002,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>mtry = 7, splitrule = gini, min.node.size = 1</t>
+          <t>mtry = 4, splitrule = gini, min.node.size = 3</t>
         </is>
       </c>
     </row>
@@ -2998,7 +3019,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>size = 9, decay = 0.1</t>
+          <t>size = 10, decay = 0.1</t>
         </is>
       </c>
     </row>
@@ -3015,7 +3036,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>sigma = 0.09, C = 3.1</t>
+          <t>sigma = 0.07, C = 3.3</t>
         </is>
       </c>
     </row>
@@ -3049,7 +3070,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>diagonal = FALSE, lambda = 0.25</t>
+          <t>diagonal = FALSE, lambda = 0.335</t>
         </is>
       </c>
     </row>
@@ -3066,7 +3087,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>mtry = 26</t>
+          <t>mtry = 9</t>
         </is>
       </c>
     </row>
@@ -3083,7 +3104,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>alpha = 0.5, lambda = 0.0158</t>
+          <t>alpha = 0.5, lambda = 0.000192</t>
         </is>
       </c>
     </row>
@@ -3149,19 +3170,19 @@
         </is>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="D2">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
       <c r="E2">
-        <v>0.15</v>
+        <v>0.28</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="3">
@@ -3182,13 +3203,13 @@
         <v>0.11</v>
       </c>
       <c r="E3">
-        <v>0.68</v>
+        <v>0.66</v>
       </c>
       <c r="F3">
-        <v>0.42</v>
+        <v>0.44</v>
       </c>
       <c r="G3">
-        <v>0.68</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="4">
@@ -3206,16 +3227,16 @@
         <v>0.47</v>
       </c>
       <c r="D4">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="E4">
-        <v>0.66</v>
+        <v>0.65</v>
       </c>
       <c r="F4">
-        <v>0.48</v>
+        <v>0.52</v>
       </c>
       <c r="G4">
-        <v>0.68</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="5">
@@ -3236,7 +3257,7 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>0.018</v>
+        <v>0.017</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -3263,13 +3284,13 @@
         <v>0.17</v>
       </c>
       <c r="E6">
-        <v>0.88</v>
+        <v>0.85</v>
       </c>
       <c r="F6">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="G6">
-        <v>0.6899999999999999</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="7">
@@ -3284,19 +3305,19 @@
         </is>
       </c>
       <c r="C7">
-        <v>0.38</v>
+        <v>0.42</v>
       </c>
       <c r="D7">
-        <v>0.078</v>
+        <v>0.13</v>
       </c>
       <c r="E7">
-        <v>0.96</v>
+        <v>0.91</v>
       </c>
       <c r="F7">
-        <v>0.33</v>
+        <v>0.44</v>
       </c>
       <c r="G7">
-        <v>0.72</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="8">
@@ -3311,19 +3332,19 @@
         </is>
       </c>
       <c r="C8">
-        <v>0.93</v>
+        <v>0.87</v>
       </c>
       <c r="D8">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="E8">
         <v>0.57</v>
       </c>
       <c r="F8">
+        <v>0.89</v>
+      </c>
+      <c r="G8">
         <v>0.88</v>
-      </c>
-      <c r="G8">
-        <v>0.99</v>
       </c>
     </row>
     <row r="9">
@@ -3338,19 +3359,19 @@
         </is>
       </c>
       <c r="C9">
-        <v>0.42</v>
+        <v>0.41</v>
       </c>
       <c r="D9">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="E9">
         <v>0.67</v>
       </c>
       <c r="F9">
-        <v>0.5600000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="G9">
-        <v>0.59</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="10">
@@ -3365,19 +3386,19 @@
         </is>
       </c>
       <c r="C10">
-        <v>0.47</v>
+        <v>0.39</v>
       </c>
       <c r="D10">
-        <v>0.21</v>
+        <v>0.09</v>
       </c>
       <c r="E10">
         <v>0.66</v>
       </c>
       <c r="F10">
-        <v>0.5600000000000001</v>
+        <v>0.48</v>
       </c>
       <c r="G10">
-        <v>0.64</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="11">
@@ -3473,13 +3494,13 @@
         </is>
       </c>
       <c r="C14">
-        <v>0.68</v>
+        <v>0.7</v>
       </c>
       <c r="D14">
-        <v>0.52</v>
+        <v>0.55</v>
       </c>
       <c r="E14">
-        <v>0.41</v>
+        <v>0.4</v>
       </c>
       <c r="F14">
         <v>0.68</v>
@@ -3500,10 +3521,10 @@
         </is>
       </c>
       <c r="C15">
-        <v>0.41</v>
+        <v>0.42</v>
       </c>
       <c r="D15">
-        <v>0.12</v>
+        <v>0.14</v>
       </c>
       <c r="E15">
         <v>0.8</v>
@@ -3512,7 +3533,7 @@
         <v>0.38</v>
       </c>
       <c r="G15">
-        <v>0.68</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="16">
@@ -3527,16 +3548,16 @@
         </is>
       </c>
       <c r="C16">
-        <v>0.39</v>
+        <v>0.43</v>
       </c>
       <c r="D16">
-        <v>0.094</v>
+        <v>0.15</v>
       </c>
       <c r="E16">
-        <v>0.74</v>
+        <v>0.76</v>
       </c>
       <c r="F16">
-        <v>0.33</v>
+        <v>0.41</v>
       </c>
       <c r="G16">
         <v>0.68</v>
@@ -3554,19 +3575,19 @@
         </is>
       </c>
       <c r="C17">
-        <v>0.7</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="D17">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="E17">
-        <v>0.55</v>
+        <v>0.58</v>
       </c>
       <c r="F17">
-        <v>0.75</v>
+        <v>0.76</v>
       </c>
       <c r="G17">
-        <v>0.84</v>
+        <v>0.8100000000000001</v>
       </c>
     </row>
     <row r="18">
@@ -3581,19 +3602,19 @@
         </is>
       </c>
       <c r="C18">
-        <v>0.38</v>
+        <v>0.4</v>
       </c>
       <c r="D18">
-        <v>0.058</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="E18">
         <v>0.66</v>
       </c>
       <c r="F18">
-        <v>0.4</v>
+        <v>0.46</v>
       </c>
       <c r="G18">
-        <v>0.67</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="19">
@@ -3608,19 +3629,19 @@
         </is>
       </c>
       <c r="C19">
-        <v>0.46</v>
+        <v>0.47</v>
       </c>
       <c r="D19">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="E19">
         <v>0.65</v>
       </c>
       <c r="F19">
-        <v>0.48</v>
+        <v>0.52</v>
       </c>
       <c r="G19">
-        <v>0.74</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="20">
@@ -3635,16 +3656,16 @@
         </is>
       </c>
       <c r="C20">
-        <v>0.72</v>
+        <v>0.75</v>
       </c>
       <c r="D20">
-        <v>0.58</v>
+        <v>0.63</v>
       </c>
       <c r="E20">
-        <v>0.41</v>
+        <v>0.33</v>
       </c>
       <c r="F20">
-        <v>0.6899999999999999</v>
+        <v>0.76</v>
       </c>
       <c r="G20">
         <v>0.86</v>
@@ -3665,13 +3686,13 @@
         <v>0.42</v>
       </c>
       <c r="D21">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="E21">
-        <v>0.76</v>
+        <v>0.99</v>
       </c>
       <c r="F21">
-        <v>0.38</v>
+        <v>0.39</v>
       </c>
       <c r="G21">
         <v>0.66</v>
@@ -3689,19 +3710,19 @@
         </is>
       </c>
       <c r="C22">
-        <v>0.38</v>
+        <v>0.32</v>
       </c>
       <c r="D22">
-        <v>0.06900000000000001</v>
+        <v>-0.014</v>
       </c>
       <c r="E22">
-        <v>0.74</v>
+        <v>1.1</v>
       </c>
       <c r="F22">
-        <v>0.41</v>
+        <v>0.33</v>
       </c>
       <c r="G22">
-        <v>0.62</v>
+        <v>0.53</v>
       </c>
     </row>
   </sheetData>
@@ -3766,19 +3787,19 @@
         </is>
       </c>
       <c r="C2">
-        <v>0.92</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>0.89</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0.42</v>
+        <v>0.16</v>
       </c>
       <c r="F2">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>0.98</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -3802,10 +3823,10 @@
         <v>0.65</v>
       </c>
       <c r="F3">
-        <v>0.48</v>
+        <v>0.5</v>
       </c>
       <c r="G3">
-        <v>0.68</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="4">
@@ -3820,19 +3841,19 @@
         </is>
       </c>
       <c r="C4">
-        <v>0.46</v>
+        <v>0.49</v>
       </c>
       <c r="D4">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
       <c r="E4">
-        <v>0.64</v>
+        <v>0.63</v>
       </c>
       <c r="F4">
         <v>0.52</v>
       </c>
       <c r="G4">
-        <v>0.7</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="5">
@@ -3847,16 +3868,16 @@
         </is>
       </c>
       <c r="C5">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>0.18</v>
+        <v>2.9e-07</v>
       </c>
       <c r="F5">
-        <v>0.91</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -3874,19 +3895,19 @@
         </is>
       </c>
       <c r="C6">
-        <v>0.48</v>
+        <v>0.47</v>
       </c>
       <c r="D6">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="E6">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>0.48</v>
+        <v>0.49</v>
       </c>
       <c r="G6">
-        <v>0.75</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="7">
@@ -3904,16 +3925,16 @@
         <v>0.42</v>
       </c>
       <c r="D7">
-        <v>0.15</v>
+        <v>0.13</v>
       </c>
       <c r="E7">
-        <v>0.92</v>
+        <v>1.1</v>
       </c>
       <c r="F7">
-        <v>0.3</v>
+        <v>0.33</v>
       </c>
       <c r="G7">
-        <v>0.85</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="8">
@@ -3928,19 +3949,19 @@
         </is>
       </c>
       <c r="C8">
-        <v>0.66</v>
+        <v>0.76</v>
       </c>
       <c r="D8">
-        <v>0.49</v>
+        <v>0.64</v>
       </c>
       <c r="E8">
-        <v>0.52</v>
+        <v>0.5</v>
       </c>
       <c r="F8">
-        <v>0.75</v>
+        <v>0.88</v>
       </c>
       <c r="G8">
-        <v>0.8</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="9">
@@ -3961,13 +3982,13 @@
         <v>0.2</v>
       </c>
       <c r="E9">
-        <v>0.63</v>
+        <v>0.64</v>
       </c>
       <c r="F9">
-        <v>0.59</v>
+        <v>0.61</v>
       </c>
       <c r="G9">
-        <v>0.68</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="10">
@@ -3982,19 +4003,19 @@
         </is>
       </c>
       <c r="C10">
-        <v>0.45</v>
+        <v>0.47</v>
       </c>
       <c r="D10">
-        <v>0.17</v>
+        <v>0.22</v>
       </c>
       <c r="E10">
         <v>0.64</v>
       </c>
       <c r="F10">
-        <v>0.48</v>
+        <v>0.52</v>
       </c>
       <c r="G10">
-        <v>0.7</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="11">
@@ -4102,7 +4123,7 @@
         <v>0.71</v>
       </c>
       <c r="G14">
-        <v>0.88</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="15">
@@ -4117,19 +4138,19 @@
         </is>
       </c>
       <c r="C15">
-        <v>0.48</v>
+        <v>0.46</v>
       </c>
       <c r="D15">
-        <v>0.22</v>
+        <v>0.19</v>
       </c>
       <c r="E15">
-        <v>0.79</v>
+        <v>0.78</v>
       </c>
       <c r="F15">
-        <v>0.42</v>
+        <v>0.45</v>
       </c>
       <c r="G15">
-        <v>0.77</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="16">
@@ -4144,16 +4165,16 @@
         </is>
       </c>
       <c r="C16">
-        <v>0.43</v>
+        <v>0.46</v>
       </c>
       <c r="D16">
-        <v>0.16</v>
+        <v>0.2</v>
       </c>
       <c r="E16">
         <v>0.76</v>
       </c>
       <c r="F16">
-        <v>0.33</v>
+        <v>0.37</v>
       </c>
       <c r="G16">
         <v>0.8100000000000001</v>
@@ -4174,16 +4195,16 @@
         <v>0.68</v>
       </c>
       <c r="D17">
-        <v>0.52</v>
+        <v>0.51</v>
       </c>
       <c r="E17">
-        <v>0.59</v>
+        <v>0.58</v>
       </c>
       <c r="F17">
-        <v>0.82</v>
+        <v>0.76</v>
       </c>
       <c r="G17">
-        <v>0.79</v>
+        <v>0.8100000000000001</v>
       </c>
     </row>
     <row r="18">
@@ -4207,10 +4228,10 @@
         <v>0.65</v>
       </c>
       <c r="F18">
-        <v>0.5600000000000001</v>
+        <v>0.55</v>
       </c>
       <c r="G18">
-        <v>0.62</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="19">
@@ -4225,16 +4246,16 @@
         </is>
       </c>
       <c r="C19">
-        <v>0.39</v>
+        <v>0.38</v>
       </c>
       <c r="D19">
-        <v>0.098</v>
+        <v>0.079</v>
       </c>
       <c r="E19">
         <v>0.65</v>
       </c>
       <c r="F19">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
       <c r="G19">
         <v>0.68</v>
@@ -4252,19 +4273,19 @@
         </is>
       </c>
       <c r="C20">
-        <v>0.8100000000000001</v>
+        <v>0.85</v>
       </c>
       <c r="D20">
-        <v>0.72</v>
+        <v>0.77</v>
       </c>
       <c r="E20">
-        <v>0.31</v>
+        <v>0.24</v>
       </c>
       <c r="F20">
-        <v>0.79</v>
+        <v>0.82</v>
       </c>
       <c r="G20">
-        <v>0.9</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="21">
@@ -4279,19 +4300,19 @@
         </is>
       </c>
       <c r="C21">
-        <v>0.48</v>
+        <v>0.47</v>
       </c>
       <c r="D21">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="E21">
-        <v>0.77</v>
+        <v>0.86</v>
       </c>
       <c r="F21">
         <v>0.48</v>
       </c>
       <c r="G21">
-        <v>0.6899999999999999</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="22">
@@ -4306,19 +4327,19 @@
         </is>
       </c>
       <c r="C22">
-        <v>0.39</v>
+        <v>0.38</v>
       </c>
       <c r="D22">
-        <v>0.1</v>
+        <v>0.074</v>
       </c>
       <c r="E22">
-        <v>0.8100000000000001</v>
+        <v>0.97</v>
       </c>
       <c r="F22">
-        <v>0.3</v>
+        <v>0.33</v>
       </c>
       <c r="G22">
-        <v>0.74</v>
+        <v>0.68</v>
       </c>
     </row>
   </sheetData>
@@ -4961,7 +4982,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>ski/snowboard/cross-country, sledding, climbing/hiking/mountaineering/skitour, biking, other</t>
+          <t>alpine skiing/snowboarding, ski touring/freeride, cross-country skiing, sledding, ice climbing, hiking, climbing, mountaineering, biking, air sport, water sport, other</t>
         </is>
       </c>
     </row>
@@ -6199,7 +6220,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>clinically relevant depression symptoms (PHQ-9 ≥11)</t>
+          <t>clinically relevant depression symptoms (PHQ-9 ≥10)</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -6941,7 +6962,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>clinically relevant depression symptoms (PHQ-9 ≥11)</t>
+          <t>clinically relevant depression symptoms (PHQ-9 ≥10)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -7400,22 +7421,36 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ski/snowboard/cross-country: 64% (n = 197)
+          <t>alpine skiing/snowboarding: 59% (n = 180)
+ski touring/freeride: 2.9% (n = 9)
+cross-country skiing: 5.5% (n = 17)
 sledding: 3.9% (n = 12)
-climbing/hiking/mountaineering/skitour: 14% (n = 42)
+ice climbing: 0.33% (n = 1)
+hiking: 5.5% (n = 17)
+climbing: 3.6% (n = 11)
+mountaineering: 0.65% (n = 2)
 biking: 16% (n = 48)
-other: 2.6% (n = 8)
+air sport: 0.33% (n = 1)
+water sport: 1.6% (n = 5)
+other: 1.3% (n = 4)
 n = 307</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ski/snowboard/cross-country: 52% (n = 2179)
-sledding: 5% (n = 207)
-climbing/hiking/mountaineering/skitour: 11% (n = 457)
+          <t>alpine skiing/snowboarding: 50% (n = 2089)
+ski touring/freeride: 2.5% (n = 105)
+cross-country skiing: 2.1% (n = 87)
+sledding: 4.8% (n = 198)
+ice climbing: 0.14% (n = 6)
+hiking: 5.1% (n = 211)
+climbing: 2.6% (n = 110)
+mountaineering: 0.41% (n = 17)
 biking: 27% (n = 1127)
-other: 4.8% (n = 202)
-n = 4172</t>
+air sport: 0.17% (n = 7)
+water sport: 1.7% (n = 72)
+other: 3.3% (n = 139)
+n = 4168</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -7425,7 +7460,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>V = 0.078</t>
+          <t>V = 0.094</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Figure and Table update
</commit_message>
<xml_diff>
--- a/paper/supplementary_tables.xlsx
+++ b/paper/supplementary_tables.xlsx
@@ -705,7 +705,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>p = 0.0083</t>
+          <t>p = 0.0078</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -737,7 +737,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>p = 0.012</t>
+          <t>p = 0.011</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -985,7 +985,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>clinically relevant somatizaton symptoms (PHQ-15 ≥11)</t>
+          <t>clinically relevant somatizaton symptoms (PHQ-15 ≥10)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1000,17 +1000,17 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>10% (n = 11)</t>
+          <t>13% (n = 14)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>p = 0.023</t>
+          <t>p = 0.0027</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>V = 0.18</t>
+          <t>V = 0.22</t>
         </is>
       </c>
     </row>
@@ -1603,7 +1603,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>p = 0.013</t>
+          <t>p = 0.012</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1851,18 +1851,18 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>alpine skiing/snowboarding: 55% (n = 57)
-ski touring/freeride: 1.9% (n = 2)
-cross-country skiing: 6.8% (n = 7)
+          <t>alpine skiing/snowboarding: 56% (n = 57)
+ski touring/freeride: 2% (n = 2)
+cross-country skiing: 6.9% (n = 7)
 sledding: 4.9% (n = 5)
 ice climbing: 0% (n = 0)
 hiking: 3.9% (n = 4)
 climbing: 2.9% (n = 3)
-mountaineering: 0.97% (n = 1)
-biking: 20% (n = 21)
-air sport: 0.97% (n = 1)
-water sport: 0.97% (n = 1)
-other: 0.97% (n = 1)</t>
+mountaineering: 0.98% (n = 1)
+biking: 21% (n = 21)
+air sports: 0.98% (n = 1)
+water sports: 0% (n = 0)
+other: 0.98% (n = 1)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1876,35 +1876,35 @@
 climbing: 2.1% (n = 2)
 mountaineering: 0% (n = 0)
 biking: 13% (n = 12)
-air sport: 0% (n = 0)
-water sport: 1.1% (n = 1)
+air sports: 0% (n = 0)
+water sports: 1.1% (n = 1)
 other: 1.1% (n = 1)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>alpine skiing/snowboarding: 56% (n = 62)
-ski touring/freeride: 3.6% (n = 4)
-cross-country skiing: 4.5% (n = 5)
-sledding: 4.5% (n = 5)
+          <t>alpine skiing/snowboarding: 58% (n = 62)
+ski touring/freeride: 3.7% (n = 4)
+cross-country skiing: 4.7% (n = 5)
+sledding: 4.7% (n = 5)
 ice climbing: 0% (n = 0)
-hiking: 6.4% (n = 7)
-climbing: 5.5% (n = 6)
-mountaineering: 0.91% (n = 1)
+hiking: 6.5% (n = 7)
+climbing: 5.6% (n = 6)
+mountaineering: 0.93% (n = 1)
 biking: 14% (n = 15)
-air sport: 0% (n = 0)
-water sport: 2.7% (n = 3)
-other: 1.8% (n = 2)</t>
+air sports: 0% (n = 0)
+water sports: 0% (n = 0)
+other: 1.9% (n = 2)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>ns (p = 0.92)</t>
+          <t>ns (p = 0.88)</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>V = 0.15</t>
+          <t>V = 0.16</t>
         </is>
       </c>
     </row>
@@ -2648,7 +2648,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>p = 0.0036</t>
+          <t>p = 0.0033</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -2883,7 +2883,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>mtry = 37, splitrule = extratrees, min.node.size = 5</t>
+          <t>mtry = 46, splitrule = extratrees, min.node.size = 1</t>
         </is>
       </c>
     </row>
@@ -2900,7 +2900,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>size = 6, decay = 1e-04</t>
+          <t>size = 9, decay = 0.01</t>
         </is>
       </c>
     </row>
@@ -2917,7 +2917,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>sigma = 0.02, C = 3.7</t>
+          <t>sigma = 0.07, C = 2.5</t>
         </is>
       </c>
     </row>
@@ -2934,7 +2934,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>cp = 0.0325</t>
+          <t>cp = 0.045</t>
         </is>
       </c>
     </row>
@@ -2951,7 +2951,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>diagonal = FALSE, lambda = 0.335</t>
+          <t>diagonal = FALSE, lambda = 0.1</t>
         </is>
       </c>
     </row>
@@ -2968,7 +2968,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>mtry = 7</t>
+          <t>mtry = 11</t>
         </is>
       </c>
     </row>
@@ -2985,7 +2985,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>alpha = 0.5, lambda = 0.00395</t>
+          <t>alpha = 0.5, lambda = 0.0149</t>
         </is>
       </c>
     </row>
@@ -3002,7 +3002,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>mtry = 4, splitrule = gini, min.node.size = 3</t>
+          <t>mtry = 9, splitrule = extratrees, min.node.size = 5</t>
         </is>
       </c>
     </row>
@@ -3019,7 +3019,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>size = 10, decay = 0.1</t>
+          <t>size = 8, decay = 0.01</t>
         </is>
       </c>
     </row>
@@ -3036,7 +3036,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>sigma = 0.07, C = 3.3</t>
+          <t>sigma = 0.01, C = 0.3</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>cp = 0.0125</t>
+          <t>cp = 0.025</t>
         </is>
       </c>
     </row>
@@ -3070,7 +3070,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>diagonal = FALSE, lambda = 0.335</t>
+          <t>diagonal = FALSE, lambda = 0.99</t>
         </is>
       </c>
     </row>
@@ -3087,7 +3087,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>mtry = 9</t>
+          <t>mtry = 6</t>
         </is>
       </c>
     </row>
@@ -3104,7 +3104,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>alpha = 0.5, lambda = 0.000192</t>
+          <t>alpha = 0.5, lambda = 0.0291</t>
         </is>
       </c>
     </row>
@@ -3176,7 +3176,7 @@
         <v>0.98</v>
       </c>
       <c r="E2">
-        <v>0.28</v>
+        <v>0.23</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -3197,19 +3197,19 @@
         </is>
       </c>
       <c r="C3">
-        <v>0.41</v>
+        <v>0.42</v>
       </c>
       <c r="D3">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="E3">
-        <v>0.66</v>
+        <v>0.67</v>
       </c>
       <c r="F3">
-        <v>0.44</v>
+        <v>0.42</v>
       </c>
       <c r="G3">
-        <v>0.66</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="4">
@@ -3224,19 +3224,19 @@
         </is>
       </c>
       <c r="C4">
-        <v>0.47</v>
+        <v>0.46</v>
       </c>
       <c r="D4">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="E4">
-        <v>0.65</v>
+        <v>0.66</v>
       </c>
       <c r="F4">
-        <v>0.52</v>
+        <v>0.46</v>
       </c>
       <c r="G4">
-        <v>0.72</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="5">
@@ -3257,7 +3257,7 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>0.017</v>
+        <v>0.0003</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -3281,16 +3281,16 @@
         <v>0.45</v>
       </c>
       <c r="D6">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="E6">
-        <v>0.85</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="F6">
-        <v>0.4</v>
+        <v>0.47</v>
       </c>
       <c r="G6">
-        <v>0.68</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="7">
@@ -3305,19 +3305,19 @@
         </is>
       </c>
       <c r="C7">
-        <v>0.42</v>
+        <v>0.39</v>
       </c>
       <c r="D7">
-        <v>0.13</v>
+        <v>0.092</v>
       </c>
       <c r="E7">
-        <v>0.91</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>0.44</v>
+        <v>0.31</v>
       </c>
       <c r="G7">
-        <v>0.57</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="8">
@@ -3332,19 +3332,19 @@
         </is>
       </c>
       <c r="C8">
-        <v>0.87</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="D8">
-        <v>0.8</v>
+        <v>0.34</v>
       </c>
       <c r="E8">
-        <v>0.57</v>
+        <v>0.58</v>
       </c>
       <c r="F8">
-        <v>0.89</v>
+        <v>0.58</v>
       </c>
       <c r="G8">
-        <v>0.88</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="9">
@@ -3359,19 +3359,19 @@
         </is>
       </c>
       <c r="C9">
-        <v>0.41</v>
+        <v>0.42</v>
       </c>
       <c r="D9">
-        <v>0.11</v>
+        <v>0.15</v>
       </c>
       <c r="E9">
-        <v>0.67</v>
+        <v>0.66</v>
       </c>
       <c r="F9">
-        <v>0.5</v>
+        <v>0.38</v>
       </c>
       <c r="G9">
-        <v>0.6</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="10">
@@ -3386,19 +3386,19 @@
         </is>
       </c>
       <c r="C10">
-        <v>0.39</v>
+        <v>0.38</v>
       </c>
       <c r="D10">
-        <v>0.09</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E10">
-        <v>0.66</v>
+        <v>0.67</v>
       </c>
       <c r="F10">
-        <v>0.48</v>
+        <v>0.35</v>
       </c>
       <c r="G10">
-        <v>0.6</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="11">
@@ -3413,19 +3413,19 @@
         </is>
       </c>
       <c r="C11">
-        <v>0.64</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="D11">
-        <v>0.45</v>
+        <v>0.33</v>
       </c>
       <c r="E11">
-        <v>0.5</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F11">
-        <v>0.62</v>
+        <v>0.65</v>
       </c>
       <c r="G11">
-        <v>0.84</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="12">
@@ -3440,19 +3440,19 @@
         </is>
       </c>
       <c r="C12">
-        <v>0.38</v>
+        <v>0.4</v>
       </c>
       <c r="D12">
-        <v>0.07000000000000001</v>
+        <v>0.094</v>
       </c>
       <c r="E12">
-        <v>0.77</v>
+        <v>0.7</v>
       </c>
       <c r="F12">
-        <v>0.38</v>
+        <v>0.44</v>
       </c>
       <c r="G12">
-        <v>0.76</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="13">
@@ -3467,16 +3467,16 @@
         </is>
       </c>
       <c r="C13">
-        <v>0.34</v>
+        <v>0.39</v>
       </c>
       <c r="D13">
-        <v>0.018</v>
+        <v>0.1</v>
       </c>
       <c r="E13">
-        <v>0.78</v>
+        <v>0.72</v>
       </c>
       <c r="F13">
-        <v>0.33</v>
+        <v>0.38</v>
       </c>
       <c r="G13">
         <v>0.7</v>
@@ -3494,19 +3494,19 @@
         </is>
       </c>
       <c r="C14">
-        <v>0.7</v>
+        <v>0.61</v>
       </c>
       <c r="D14">
-        <v>0.55</v>
+        <v>0.42</v>
       </c>
       <c r="E14">
-        <v>0.4</v>
+        <v>0.54</v>
       </c>
       <c r="F14">
-        <v>0.68</v>
+        <v>0.54</v>
       </c>
       <c r="G14">
-        <v>0.87</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="15">
@@ -3524,16 +3524,16 @@
         <v>0.42</v>
       </c>
       <c r="D15">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="E15">
-        <v>0.8</v>
+        <v>0.86</v>
       </c>
       <c r="F15">
-        <v>0.38</v>
+        <v>0.36</v>
       </c>
       <c r="G15">
-        <v>0.71</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="16">
@@ -3548,19 +3548,19 @@
         </is>
       </c>
       <c r="C16">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="D16">
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
       <c r="E16">
-        <v>0.76</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="F16">
-        <v>0.41</v>
+        <v>0.38</v>
       </c>
       <c r="G16">
-        <v>0.68</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="17">
@@ -3575,19 +3575,19 @@
         </is>
       </c>
       <c r="C17">
-        <v>0.6899999999999999</v>
+        <v>0.65</v>
       </c>
       <c r="D17">
-        <v>0.54</v>
+        <v>0.47</v>
       </c>
       <c r="E17">
-        <v>0.58</v>
+        <v>0.59</v>
       </c>
       <c r="F17">
-        <v>0.76</v>
+        <v>0.71</v>
       </c>
       <c r="G17">
-        <v>0.8100000000000001</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="18">
@@ -3605,13 +3605,13 @@
         <v>0.4</v>
       </c>
       <c r="D18">
-        <v>0.08799999999999999</v>
+        <v>0.094</v>
       </c>
       <c r="E18">
         <v>0.66</v>
       </c>
       <c r="F18">
-        <v>0.46</v>
+        <v>0.47</v>
       </c>
       <c r="G18">
         <v>0.64</v>
@@ -3629,19 +3629,19 @@
         </is>
       </c>
       <c r="C19">
-        <v>0.47</v>
+        <v>0.42</v>
       </c>
       <c r="D19">
-        <v>0.21</v>
+        <v>0.14</v>
       </c>
       <c r="E19">
-        <v>0.65</v>
+        <v>0.66</v>
       </c>
       <c r="F19">
-        <v>0.52</v>
+        <v>0.46</v>
       </c>
       <c r="G19">
-        <v>0.66</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="20">
@@ -3656,19 +3656,19 @@
         </is>
       </c>
       <c r="C20">
-        <v>0.75</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="D20">
+        <v>0.53</v>
+      </c>
+      <c r="E20">
+        <v>0.44</v>
+      </c>
+      <c r="F20">
         <v>0.63</v>
       </c>
-      <c r="E20">
-        <v>0.33</v>
-      </c>
-      <c r="F20">
-        <v>0.76</v>
-      </c>
       <c r="G20">
-        <v>0.86</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="21">
@@ -3683,19 +3683,19 @@
         </is>
       </c>
       <c r="C21">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
       <c r="D21">
-        <v>0.12</v>
+        <v>0.19</v>
       </c>
       <c r="E21">
-        <v>0.99</v>
+        <v>0.73</v>
       </c>
       <c r="F21">
-        <v>0.39</v>
+        <v>0.41</v>
       </c>
       <c r="G21">
-        <v>0.66</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="22">
@@ -3710,19 +3710,19 @@
         </is>
       </c>
       <c r="C22">
-        <v>0.32</v>
+        <v>0.39</v>
       </c>
       <c r="D22">
-        <v>-0.014</v>
+        <v>0.091</v>
       </c>
       <c r="E22">
-        <v>1.1</v>
+        <v>0.7</v>
       </c>
       <c r="F22">
-        <v>0.33</v>
+        <v>0.46</v>
       </c>
       <c r="G22">
-        <v>0.53</v>
+        <v>0.65</v>
       </c>
     </row>
   </sheetData>
@@ -3793,7 +3793,7 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>0.16</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -3814,19 +3814,19 @@
         </is>
       </c>
       <c r="C3">
-        <v>0.43</v>
+        <v>0.46</v>
       </c>
       <c r="D3">
-        <v>0.14</v>
+        <v>0.19</v>
       </c>
       <c r="E3">
-        <v>0.65</v>
+        <v>0.64</v>
       </c>
       <c r="F3">
-        <v>0.5</v>
+        <v>0.47</v>
       </c>
       <c r="G3">
-        <v>0.66</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="4">
@@ -3841,19 +3841,19 @@
         </is>
       </c>
       <c r="C4">
-        <v>0.49</v>
+        <v>0.46</v>
       </c>
       <c r="D4">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
       <c r="E4">
-        <v>0.63</v>
+        <v>0.64</v>
       </c>
       <c r="F4">
-        <v>0.52</v>
+        <v>0.46</v>
       </c>
       <c r="G4">
-        <v>0.79</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="5">
@@ -3874,7 +3874,7 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>2.9e-07</v>
+        <v>0.00021</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -3901,13 +3901,13 @@
         <v>0.2</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0.92</v>
       </c>
       <c r="F6">
-        <v>0.49</v>
+        <v>0.42</v>
       </c>
       <c r="G6">
-        <v>0.72</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="7">
@@ -3922,19 +3922,19 @@
         </is>
       </c>
       <c r="C7">
-        <v>0.42</v>
+        <v>0.36</v>
       </c>
       <c r="D7">
-        <v>0.13</v>
+        <v>0.055</v>
       </c>
       <c r="E7">
         <v>1.1</v>
       </c>
       <c r="F7">
-        <v>0.33</v>
+        <v>0.27</v>
       </c>
       <c r="G7">
-        <v>0.68</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="8">
@@ -3949,19 +3949,19 @@
         </is>
       </c>
       <c r="C8">
-        <v>0.76</v>
+        <v>0.96</v>
       </c>
       <c r="D8">
-        <v>0.64</v>
+        <v>0.95</v>
       </c>
       <c r="E8">
-        <v>0.5</v>
+        <v>0.34</v>
       </c>
       <c r="F8">
-        <v>0.88</v>
+        <v>0.97</v>
       </c>
       <c r="G8">
-        <v>0.84</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="9">
@@ -3976,19 +3976,19 @@
         </is>
       </c>
       <c r="C9">
-        <v>0.47</v>
+        <v>0.46</v>
       </c>
       <c r="D9">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="E9">
+        <v>0.65</v>
+      </c>
+      <c r="F9">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="G9">
         <v>0.64</v>
-      </c>
-      <c r="F9">
-        <v>0.61</v>
-      </c>
-      <c r="G9">
-        <v>0.62</v>
       </c>
     </row>
     <row r="10">
@@ -4003,19 +4003,19 @@
         </is>
       </c>
       <c r="C10">
-        <v>0.47</v>
+        <v>0.44</v>
       </c>
       <c r="D10">
-        <v>0.22</v>
+        <v>0.17</v>
       </c>
       <c r="E10">
-        <v>0.64</v>
+        <v>0.66</v>
       </c>
       <c r="F10">
-        <v>0.52</v>
+        <v>0.46</v>
       </c>
       <c r="G10">
-        <v>0.74</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="11">
@@ -4030,19 +4030,19 @@
         </is>
       </c>
       <c r="C11">
-        <v>0.54</v>
+        <v>0.48</v>
       </c>
       <c r="D11">
-        <v>0.32</v>
+        <v>0.21</v>
       </c>
       <c r="E11">
-        <v>0.57</v>
+        <v>0.61</v>
       </c>
       <c r="F11">
-        <v>0.55</v>
+        <v>0.65</v>
       </c>
       <c r="G11">
-        <v>0.79</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="12">
@@ -4057,19 +4057,19 @@
         </is>
       </c>
       <c r="C12">
-        <v>0.38</v>
+        <v>0.43</v>
       </c>
       <c r="D12">
-        <v>0.059</v>
+        <v>0.13</v>
       </c>
       <c r="E12">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="F12">
-        <v>0.39</v>
+        <v>0.49</v>
       </c>
       <c r="G12">
-        <v>0.66</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="13">
@@ -4087,16 +4087,16 @@
         <v>0.36</v>
       </c>
       <c r="D13">
-        <v>0.049</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="E13">
-        <v>0.7</v>
+        <v>0.66</v>
       </c>
       <c r="F13">
-        <v>0.41</v>
+        <v>0.42</v>
       </c>
       <c r="G13">
-        <v>0.72</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="14">
@@ -4111,16 +4111,16 @@
         </is>
       </c>
       <c r="C14">
-        <v>0.76</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="D14">
-        <v>0.64</v>
+        <v>0.71</v>
       </c>
       <c r="E14">
-        <v>0.34</v>
+        <v>0.3</v>
       </c>
       <c r="F14">
-        <v>0.71</v>
+        <v>0.78</v>
       </c>
       <c r="G14">
         <v>0.9</v>
@@ -4138,19 +4138,19 @@
         </is>
       </c>
       <c r="C15">
+        <v>0.47</v>
+      </c>
+      <c r="D15">
+        <v>0.21</v>
+      </c>
+      <c r="E15">
+        <v>0.82</v>
+      </c>
+      <c r="F15">
         <v>0.46</v>
       </c>
-      <c r="D15">
-        <v>0.19</v>
-      </c>
-      <c r="E15">
-        <v>0.78</v>
-      </c>
-      <c r="F15">
-        <v>0.45</v>
-      </c>
       <c r="G15">
-        <v>0.75</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="16">
@@ -4165,19 +4165,19 @@
         </is>
       </c>
       <c r="C16">
-        <v>0.46</v>
+        <v>0.44</v>
       </c>
       <c r="D16">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="E16">
-        <v>0.76</v>
+        <v>0.84</v>
       </c>
       <c r="F16">
-        <v>0.37</v>
+        <v>0.35</v>
       </c>
       <c r="G16">
-        <v>0.8100000000000001</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="17">
@@ -4192,16 +4192,16 @@
         </is>
       </c>
       <c r="C17">
-        <v>0.68</v>
+        <v>0.67</v>
       </c>
       <c r="D17">
         <v>0.51</v>
       </c>
       <c r="E17">
-        <v>0.58</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F17">
-        <v>0.76</v>
+        <v>0.77</v>
       </c>
       <c r="G17">
         <v>0.8100000000000001</v>
@@ -4219,19 +4219,19 @@
         </is>
       </c>
       <c r="C18">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="D18">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="E18">
-        <v>0.65</v>
+        <v>0.64</v>
       </c>
       <c r="F18">
-        <v>0.55</v>
+        <v>0.51</v>
       </c>
       <c r="G18">
-        <v>0.66</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="19">
@@ -4246,19 +4246,19 @@
         </is>
       </c>
       <c r="C19">
-        <v>0.38</v>
+        <v>0.39</v>
       </c>
       <c r="D19">
-        <v>0.079</v>
+        <v>0.1</v>
       </c>
       <c r="E19">
-        <v>0.65</v>
+        <v>0.66</v>
       </c>
       <c r="F19">
-        <v>0.44</v>
+        <v>0.42</v>
       </c>
       <c r="G19">
-        <v>0.68</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="20">
@@ -4273,19 +4273,19 @@
         </is>
       </c>
       <c r="C20">
-        <v>0.85</v>
+        <v>0.82</v>
       </c>
       <c r="D20">
-        <v>0.77</v>
+        <v>0.72</v>
       </c>
       <c r="E20">
-        <v>0.24</v>
+        <v>0.32</v>
       </c>
       <c r="F20">
-        <v>0.82</v>
+        <v>0.79</v>
       </c>
       <c r="G20">
-        <v>0.92</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="21">
@@ -4300,19 +4300,19 @@
         </is>
       </c>
       <c r="C21">
-        <v>0.47</v>
+        <v>0.49</v>
       </c>
       <c r="D21">
-        <v>0.21</v>
+        <v>0.23</v>
       </c>
       <c r="E21">
-        <v>0.86</v>
+        <v>0.74</v>
       </c>
       <c r="F21">
-        <v>0.48</v>
+        <v>0.49</v>
       </c>
       <c r="G21">
-        <v>0.66</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="22">
@@ -4327,19 +4327,19 @@
         </is>
       </c>
       <c r="C22">
-        <v>0.38</v>
+        <v>0.42</v>
       </c>
       <c r="D22">
-        <v>0.074</v>
+        <v>0.14</v>
       </c>
       <c r="E22">
-        <v>0.97</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="F22">
-        <v>0.33</v>
+        <v>0.31</v>
       </c>
       <c r="G22">
-        <v>0.68</v>
+        <v>0.78</v>
       </c>
     </row>
   </sheetData>
@@ -4982,7 +4982,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>alpine skiing/snowboarding, ski touring/freeride, cross-country skiing, sledding, ice climbing, hiking, climbing, mountaineering, biking, air sport, water sport, other</t>
+          <t>alpine skiing/snowboarding, ski touring/freeride, cross-country skiing, sledding, ice climbing, hiking, climbing, mountaineering, biking, air sports, water sports, other</t>
         </is>
       </c>
     </row>
@@ -6225,7 +6225,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>PHQ-9 score ≥ 11 points, clinically relevant depressive symptoms</t>
+          <t>PHQ-9 score ≥ 10 points, clinically relevant depressive symptoms</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -6367,12 +6367,12 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>clinically relevant somatizaton symptoms (PHQ-15 ≥11)</t>
+          <t>clinically relevant somatizaton symptoms (PHQ-15 ≥10)</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>PHQ-15 score ≥ 11 points, clinically relevant somatization symptoms</t>
+          <t>PHQ-15 score ≥ 10 points, clinically relevant somatization symptoms</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -6967,7 +6967,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>PHQ-9 score ≥ 11 points, clinically relevant depressive symptoms</t>
+          <t>PHQ-9 score ≥ 10 points, clinically relevant depressive symptoms</t>
         </is>
       </c>
     </row>
@@ -7064,12 +7064,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>clinically relevant somatizaton symptoms (PHQ-15 ≥11)</t>
+          <t>clinically relevant somatizaton symptoms (PHQ-15 ≥10)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>PHQ-15 score ≥ 11 points, clinically relevant somatization symptoms</t>
+          <t>PHQ-15 score ≥ 10 points, clinically relevant somatization symptoms</t>
         </is>
       </c>
     </row>
@@ -7422,35 +7422,35 @@
       <c r="B2" t="inlineStr">
         <is>
           <t>alpine skiing/snowboarding: 59% (n = 180)
-ski touring/freeride: 2.9% (n = 9)
-cross-country skiing: 5.5% (n = 17)
-sledding: 3.9% (n = 12)
+ski touring/freeride: 3% (n = 9)
+cross-country skiing: 5.6% (n = 17)
+sledding: 4% (n = 12)
 ice climbing: 0.33% (n = 1)
-hiking: 5.5% (n = 17)
+hiking: 5.6% (n = 17)
 climbing: 3.6% (n = 11)
-mountaineering: 0.65% (n = 2)
+mountaineering: 0.66% (n = 2)
 biking: 16% (n = 48)
-air sport: 0.33% (n = 1)
-water sport: 1.6% (n = 5)
+air sports: 0.33% (n = 1)
+water sports: 0.33% (n = 1)
 other: 1.3% (n = 4)
-n = 307</t>
+n = 303</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>alpine skiing/snowboarding: 50% (n = 2089)
-ski touring/freeride: 2.5% (n = 105)
+          <t>alpine skiing/snowboarding: 51% (n = 2089)
+ski touring/freeride: 2.6% (n = 105)
 cross-country skiing: 2.1% (n = 87)
 sledding: 4.8% (n = 198)
-ice climbing: 0.14% (n = 6)
+ice climbing: 0.15% (n = 6)
 hiking: 5.1% (n = 211)
-climbing: 2.6% (n = 110)
+climbing: 2.7% (n = 110)
 mountaineering: 0.41% (n = 17)
 biking: 27% (n = 1127)
-air sport: 0.17% (n = 7)
-water sport: 1.7% (n = 72)
-other: 3.3% (n = 139)
-n = 4168</t>
+air sports: 0.17% (n = 7)
+water sports: 0.15% (n = 6)
+other: 3.4% (n = 139)
+n = 4102</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -7460,7 +7460,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>V = 0.094</t>
+          <t>V = 0.096</t>
         </is>
       </c>
     </row>

</xml_diff>